<commit_message>
Further data entry for FY21/22 & Q breakdown
</commit_message>
<xml_diff>
--- a/$TWLO.xlsx
+++ b/$TWLO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\me\Documents\Google Drive\Stocks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94A26BCA-A8B4-4561-988C-25ECDF6CF549}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7476CCB-A0C6-4FF0-A592-3014EEA9B614}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" activeTab="1" xr2:uid="{1EC168B4-1311-4642-A238-D70265844B27}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1730" uniqueCount="1716">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1742" uniqueCount="1717">
   <si>
     <t>$TWLO</t>
   </si>
@@ -5175,6 +5175,9 @@
   </si>
   <si>
     <t>Y/Y</t>
+  </si>
+  <si>
+    <t>-</t>
   </si>
 </sst>
 </file>
@@ -5378,7 +5381,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -5446,6 +5449,23 @@
     <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="3" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="9" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -5473,23 +5493,10 @@
     <xf numFmtId="0" fontId="7" fillId="4" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="3" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="9" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="166" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -11234,6 +11241,111 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>84</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="3" name="Straight Connector 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{66ED336B-143B-490D-898B-F8B180976103}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12601575" y="9525"/>
+          <a:ext cx="0" cy="13668375"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>84</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="5" name="Straight Connector 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E99DBC6E-145A-400A-87C4-2B34A2A31C5C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="17535525" y="0"/>
+          <a:ext cx="0" cy="13668375"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -11534,7 +11646,7 @@
   <dimension ref="B2:S35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="S2" sqref="S2"/>
+      <selection activeCell="P33" sqref="P33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -11557,24 +11669,24 @@
       </c>
     </row>
     <row r="5" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B5" s="39" t="s">
+      <c r="B5" s="50" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="40"/>
-      <c r="D5" s="41"/>
-      <c r="G5" s="39" t="s">
+      <c r="C5" s="51"/>
+      <c r="D5" s="52"/>
+      <c r="G5" s="50" t="s">
         <v>24</v>
       </c>
-      <c r="H5" s="40"/>
-      <c r="I5" s="40"/>
-      <c r="J5" s="40"/>
-      <c r="K5" s="40"/>
-      <c r="L5" s="40"/>
-      <c r="M5" s="40"/>
-      <c r="N5" s="40"/>
-      <c r="O5" s="40"/>
-      <c r="P5" s="40"/>
-      <c r="Q5" s="41"/>
+      <c r="H5" s="51"/>
+      <c r="I5" s="51"/>
+      <c r="J5" s="51"/>
+      <c r="K5" s="51"/>
+      <c r="L5" s="51"/>
+      <c r="M5" s="51"/>
+      <c r="N5" s="51"/>
+      <c r="O5" s="51"/>
+      <c r="P5" s="51"/>
+      <c r="Q5" s="52"/>
     </row>
     <row r="6" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B6" s="5" t="s">
@@ -11761,11 +11873,11 @@
       <c r="Q14" s="9"/>
     </row>
     <row r="15" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B15" s="39" t="s">
+      <c r="B15" s="50" t="s">
         <v>10</v>
       </c>
-      <c r="C15" s="40"/>
-      <c r="D15" s="41"/>
+      <c r="C15" s="51"/>
+      <c r="D15" s="52"/>
       <c r="G15" s="20"/>
       <c r="H15" s="8"/>
       <c r="I15" s="8"/>
@@ -11782,10 +11894,10 @@
       <c r="B16" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="C16" s="48" t="s">
+      <c r="C16" s="46" t="s">
         <v>22</v>
       </c>
-      <c r="D16" s="49"/>
+      <c r="D16" s="47"/>
       <c r="G16" s="20"/>
       <c r="H16" s="8"/>
       <c r="I16" s="8"/>
@@ -11802,8 +11914,8 @@
       <c r="B17" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C17" s="50"/>
-      <c r="D17" s="51"/>
+      <c r="C17" s="44"/>
+      <c r="D17" s="45"/>
       <c r="G17" s="20"/>
       <c r="H17" s="8"/>
       <c r="I17" s="8"/>
@@ -11820,10 +11932,10 @@
       <c r="B18" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="C18" s="48" t="s">
+      <c r="C18" s="46" t="s">
         <v>23</v>
       </c>
-      <c r="D18" s="49"/>
+      <c r="D18" s="47"/>
       <c r="G18" s="20"/>
       <c r="H18" s="8"/>
       <c r="I18" s="8"/>
@@ -11840,8 +11952,8 @@
       <c r="B19" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="C19" s="52"/>
-      <c r="D19" s="53"/>
+      <c r="C19" s="48"/>
+      <c r="D19" s="49"/>
       <c r="G19" s="20"/>
       <c r="H19" s="8"/>
       <c r="I19" s="8"/>
@@ -11881,11 +11993,11 @@
       <c r="Q21" s="9"/>
     </row>
     <row r="22" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B22" s="39" t="s">
+      <c r="B22" s="50" t="s">
         <v>15</v>
       </c>
-      <c r="C22" s="40"/>
-      <c r="D22" s="41"/>
+      <c r="C22" s="51"/>
+      <c r="D22" s="52"/>
       <c r="G22" s="20"/>
       <c r="H22" s="8"/>
       <c r="I22" s="8"/>
@@ -11902,10 +12014,10 @@
       <c r="B23" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="C23" s="48" t="s">
+      <c r="C23" s="46" t="s">
         <v>21</v>
       </c>
-      <c r="D23" s="49"/>
+      <c r="D23" s="47"/>
       <c r="G23" s="20"/>
       <c r="H23" s="8"/>
       <c r="I23" s="8"/>
@@ -11922,10 +12034,10 @@
       <c r="B24" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="C24" s="48">
+      <c r="C24" s="46">
         <v>2008</v>
       </c>
-      <c r="D24" s="49"/>
+      <c r="D24" s="47"/>
       <c r="G24" s="20"/>
       <c r="H24" s="8"/>
       <c r="I24" s="8"/>
@@ -11940,8 +12052,8 @@
     </row>
     <row r="25" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B25" s="13"/>
-      <c r="C25" s="48"/>
-      <c r="D25" s="49"/>
+      <c r="C25" s="46"/>
+      <c r="D25" s="47"/>
       <c r="G25" s="20"/>
       <c r="H25" s="8"/>
       <c r="I25" s="8"/>
@@ -11956,8 +12068,8 @@
     </row>
     <row r="26" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B26" s="13"/>
-      <c r="C26" s="48"/>
-      <c r="D26" s="49"/>
+      <c r="C26" s="46"/>
+      <c r="D26" s="47"/>
       <c r="G26" s="20"/>
       <c r="H26" s="8"/>
       <c r="I26" s="8"/>
@@ -11972,8 +12084,8 @@
     </row>
     <row r="27" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B27" s="13"/>
-      <c r="C27" s="48"/>
-      <c r="D27" s="49"/>
+      <c r="C27" s="46"/>
+      <c r="D27" s="47"/>
       <c r="G27" s="20"/>
       <c r="H27" s="8"/>
       <c r="I27" s="8"/>
@@ -12013,10 +12125,10 @@
       <c r="B29" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="C29" s="46" t="s">
+      <c r="C29" s="57" t="s">
         <v>20</v>
       </c>
-      <c r="D29" s="47"/>
+      <c r="D29" s="58"/>
       <c r="G29" s="21"/>
       <c r="H29" s="11"/>
       <c r="I29" s="11"/>
@@ -12030,51 +12142,44 @@
       <c r="Q29" s="12"/>
     </row>
     <row r="32" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B32" s="39" t="s">
+      <c r="B32" s="50" t="s">
         <v>106</v>
       </c>
-      <c r="C32" s="40"/>
-      <c r="D32" s="41"/>
+      <c r="C32" s="51"/>
+      <c r="D32" s="52"/>
     </row>
     <row r="33" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B33" s="13" t="s">
         <v>103</v>
       </c>
-      <c r="C33" s="42">
+      <c r="C33" s="53">
         <f>'Financial Model'!T77</f>
         <v>1.4095721757702342</v>
       </c>
-      <c r="D33" s="43"/>
+      <c r="D33" s="54"/>
     </row>
     <row r="34" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B34" s="13" t="s">
         <v>105</v>
       </c>
-      <c r="C34" s="42">
+      <c r="C34" s="53">
         <f>'Financial Model'!T78</f>
-        <v>16.200254074122757</v>
-      </c>
-      <c r="D34" s="43"/>
+        <v>4.4927117390362339</v>
+      </c>
+      <c r="D34" s="54"/>
     </row>
     <row r="35" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B35" s="14" t="s">
         <v>104</v>
       </c>
-      <c r="C35" s="44">
+      <c r="C35" s="55">
         <f>'Financial Model'!T79</f>
-        <v>-47.348334201363834</v>
-      </c>
-      <c r="D35" s="45"/>
+        <v>-14.233498713981406</v>
+      </c>
+      <c r="D35" s="56"/>
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="G5:Q5"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="B15:D15"/>
-    <mergeCell ref="C16:D16"/>
     <mergeCell ref="B32:D32"/>
     <mergeCell ref="C33:D33"/>
     <mergeCell ref="C34:D34"/>
@@ -12086,6 +12191,13 @@
     <mergeCell ref="C25:D25"/>
     <mergeCell ref="C24:D24"/>
     <mergeCell ref="C23:D23"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="G5:Q5"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="B15:D15"/>
+    <mergeCell ref="C16:D16"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C29:D29" r:id="rId1" display="Link" xr:uid="{14045B38-8430-46EA-8F9C-1AE5F20888F1}"/>
@@ -12101,10 +12213,10 @@
   <dimension ref="A1:AL79"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C12" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="S34" sqref="S34"/>
+      <selection pane="bottomRight" activeCell="O42" sqref="O42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -12159,10 +12271,10 @@
       <c r="P1" s="22" t="s">
         <v>38</v>
       </c>
-      <c r="Q1" s="22" t="s">
+      <c r="Q1" s="27" t="s">
         <v>39</v>
       </c>
-      <c r="R1" s="22" t="s">
+      <c r="R1" s="27" t="s">
         <v>40</v>
       </c>
       <c r="S1" s="27" t="s">
@@ -12186,7 +12298,7 @@
       <c r="AA1" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="AB1" s="22" t="s">
+      <c r="AB1" s="27" t="s">
         <v>48</v>
       </c>
       <c r="AC1" s="22" t="s">
@@ -12222,12 +12334,21 @@
     </row>
     <row r="2" spans="1:38" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="23"/>
+      <c r="M2" s="26">
+        <v>44104</v>
+      </c>
+      <c r="N2" s="26">
+        <v>44196</v>
+      </c>
       <c r="O2" s="26">
         <v>44286</v>
       </c>
       <c r="P2" s="26">
         <v>44377</v>
       </c>
+      <c r="Q2" s="26">
+        <v>44469</v>
+      </c>
       <c r="R2" s="26">
         <v>44561</v>
       </c>
@@ -12237,54 +12358,113 @@
       <c r="T2" s="26">
         <v>44742</v>
       </c>
+      <c r="AA2" s="26">
+        <v>44196</v>
+      </c>
+      <c r="AB2" s="26">
+        <v>44561</v>
+      </c>
     </row>
     <row r="3" spans="1:38" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="23"/>
+      <c r="Q3" s="25">
+        <v>46661</v>
+      </c>
+      <c r="R3" s="25">
+        <v>39845</v>
+      </c>
       <c r="S3" s="25">
         <v>38108</v>
       </c>
       <c r="T3" s="25">
         <v>38200</v>
+      </c>
+      <c r="AB3" s="25">
+        <v>39845</v>
       </c>
     </row>
     <row r="4" spans="1:38" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B4" s="2" t="s">
         <v>59</v>
       </c>
+      <c r="M4" s="29">
+        <v>447.96899999999999</v>
+      </c>
+      <c r="N4" s="29">
+        <v>548.09</v>
+      </c>
       <c r="O4" s="29">
         <v>589.98800000000006</v>
       </c>
       <c r="P4" s="29">
         <v>668.93100000000004</v>
       </c>
+      <c r="Q4" s="29">
+        <v>740.17600000000004</v>
+      </c>
+      <c r="R4" s="29">
+        <v>842.74400000000003</v>
+      </c>
       <c r="S4" s="29">
         <v>875.36300000000006</v>
       </c>
       <c r="T4" s="29">
         <v>943.35400000000004</v>
+      </c>
+      <c r="AA4" s="29">
+        <v>1761.7760000000001</v>
+      </c>
+      <c r="AB4" s="29">
+        <v>2841.8389999999999</v>
       </c>
     </row>
     <row r="5" spans="1:38" x14ac:dyDescent="0.2">
       <c r="B5" s="1" t="s">
         <v>60</v>
       </c>
+      <c r="M5" s="30">
+        <v>217.095</v>
+      </c>
+      <c r="N5" s="30">
+        <v>265.96899999999999</v>
+      </c>
       <c r="O5" s="30">
         <v>291.68400000000003</v>
       </c>
       <c r="P5" s="30">
         <v>337.68400000000003</v>
       </c>
+      <c r="Q5" s="30">
+        <v>375.56099999999998</v>
+      </c>
+      <c r="R5" s="30">
+        <v>446.197</v>
+      </c>
       <c r="S5" s="30">
         <v>450.29199999999997</v>
       </c>
       <c r="T5" s="30">
         <v>498.065</v>
+      </c>
+      <c r="AA5" s="30">
+        <v>846.11500000000001</v>
+      </c>
+      <c r="AB5" s="30">
+        <v>1451.126</v>
       </c>
     </row>
     <row r="6" spans="1:38" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B6" s="2" t="s">
         <v>61</v>
       </c>
+      <c r="M6" s="29">
+        <f t="shared" ref="M6" si="0">M4-M5</f>
+        <v>230.874</v>
+      </c>
+      <c r="N6" s="29">
+        <f>N4-N5</f>
+        <v>282.12100000000004</v>
+      </c>
       <c r="O6" s="29">
         <f>O4-O5</f>
         <v>298.30400000000003</v>
@@ -12293,6 +12473,14 @@
         <f>P4-P5</f>
         <v>331.24700000000001</v>
       </c>
+      <c r="Q6" s="29">
+        <f>Q4-Q5</f>
+        <v>364.61500000000007</v>
+      </c>
+      <c r="R6" s="29">
+        <f>R4-R5</f>
+        <v>396.54700000000003</v>
+      </c>
       <c r="S6" s="29">
         <f>S4-S5</f>
         <v>425.07100000000008</v>
@@ -12301,70 +12489,148 @@
         <f>T4-T5</f>
         <v>445.28900000000004</v>
       </c>
+      <c r="AA6" s="29">
+        <f>AA4-AA5</f>
+        <v>915.66100000000006</v>
+      </c>
+      <c r="AB6" s="29">
+        <f>AB4-AB5</f>
+        <v>1390.713</v>
+      </c>
     </row>
     <row r="7" spans="1:38" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
         <v>62</v>
       </c>
+      <c r="M7" s="30">
+        <v>136.65199999999999</v>
+      </c>
+      <c r="N7" s="30">
+        <v>158.85599999999999</v>
+      </c>
       <c r="O7" s="30">
         <v>174.8</v>
       </c>
       <c r="P7" s="30">
         <v>181.28</v>
       </c>
+      <c r="Q7" s="30">
+        <v>209.89</v>
+      </c>
+      <c r="R7" s="30">
+        <v>223.249</v>
+      </c>
       <c r="S7" s="30">
         <v>240.61099999999999</v>
       </c>
       <c r="T7" s="30">
         <v>279.64100000000002</v>
+      </c>
+      <c r="AA7" s="30">
+        <v>530.548</v>
+      </c>
+      <c r="AB7" s="30">
+        <v>789.21900000000005</v>
       </c>
     </row>
     <row r="8" spans="1:38" x14ac:dyDescent="0.2">
       <c r="B8" s="1" t="s">
         <v>63</v>
       </c>
+      <c r="M8" s="30">
+        <v>140.875</v>
+      </c>
+      <c r="N8" s="30">
+        <v>179.98699999999999</v>
+      </c>
       <c r="O8" s="30">
         <v>210.59</v>
       </c>
       <c r="P8" s="30">
         <v>238.05799999999999</v>
       </c>
+      <c r="Q8" s="30">
+        <v>264.548</v>
+      </c>
+      <c r="R8" s="30">
+        <v>331.42200000000003</v>
+      </c>
       <c r="S8" s="30">
         <v>287.90600000000001</v>
       </c>
       <c r="T8" s="30">
         <v>334.95800000000003</v>
+      </c>
+      <c r="AA8" s="30">
+        <v>567.40700000000004</v>
+      </c>
+      <c r="AB8" s="30">
+        <v>1044.6179999999999</v>
       </c>
     </row>
     <row r="9" spans="1:38" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s">
         <v>64</v>
       </c>
+      <c r="M9" s="30">
+        <v>65.617000000000004</v>
+      </c>
+      <c r="N9" s="30">
+        <v>128.56899999999999</v>
+      </c>
       <c r="O9" s="30">
         <v>110.253</v>
       </c>
       <c r="P9" s="30">
         <v>114.18300000000001</v>
       </c>
+      <c r="Q9" s="30">
+        <v>122.52200000000001</v>
+      </c>
+      <c r="R9" s="30">
+        <v>125.502</v>
+      </c>
       <c r="S9" s="30">
         <v>114.36199999999999</v>
       </c>
       <c r="T9" s="30">
         <v>142.626</v>
+      </c>
+      <c r="AA9" s="30">
+        <v>310.60700000000003</v>
+      </c>
+      <c r="AB9" s="30">
+        <v>472.46</v>
       </c>
     </row>
     <row r="10" spans="1:38" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
         <v>65</v>
       </c>
+      <c r="M10" s="30">
+        <f t="shared" ref="M10:O10" si="1">SUM(M7:M9)</f>
+        <v>343.14400000000001</v>
+      </c>
+      <c r="N10" s="30">
+        <f t="shared" si="1"/>
+        <v>467.41199999999992</v>
+      </c>
       <c r="O10" s="30">
-        <f t="shared" ref="O10" si="0">SUM(O7:O9)</f>
+        <f t="shared" si="1"/>
         <v>495.64299999999997</v>
       </c>
       <c r="P10" s="30">
         <f>SUM(P7:P9)</f>
         <v>533.52099999999996</v>
       </c>
+      <c r="Q10" s="30">
+        <f t="shared" ref="Q10" si="2">SUM(Q7:Q9)</f>
+        <v>596.96</v>
+      </c>
+      <c r="R10" s="30">
+        <f t="shared" ref="R10" si="3">SUM(R7:R9)</f>
+        <v>680.173</v>
+      </c>
       <c r="S10" s="30">
         <f>SUM(S7:S9)</f>
         <v>642.87900000000002</v>
@@ -12373,19 +12639,43 @@
         <f>SUM(T7:T9)</f>
         <v>757.22500000000002</v>
       </c>
+      <c r="AA10" s="30">
+        <f t="shared" ref="AA10" si="4">SUM(AA7:AA9)</f>
+        <v>1408.5619999999999</v>
+      </c>
+      <c r="AB10" s="30">
+        <f>SUM(AB7:AB9)</f>
+        <v>2306.297</v>
+      </c>
     </row>
     <row r="11" spans="1:38" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B11" s="2" t="s">
         <v>66</v>
       </c>
+      <c r="M11" s="29">
+        <f t="shared" ref="M11:O11" si="5">M6-M10</f>
+        <v>-112.27000000000001</v>
+      </c>
+      <c r="N11" s="29">
+        <f t="shared" si="5"/>
+        <v>-185.29099999999988</v>
+      </c>
       <c r="O11" s="29">
-        <f t="shared" ref="O11" si="1">O6-O10</f>
+        <f t="shared" si="5"/>
         <v>-197.33899999999994</v>
       </c>
       <c r="P11" s="29">
         <f>P6-P10</f>
         <v>-202.27399999999994</v>
       </c>
+      <c r="Q11" s="29">
+        <f t="shared" ref="Q11" si="6">Q6-Q10</f>
+        <v>-232.34499999999997</v>
+      </c>
+      <c r="R11" s="29">
+        <f t="shared" ref="R11" si="7">R6-R10</f>
+        <v>-283.62599999999998</v>
+      </c>
       <c r="S11" s="29">
         <f>S6-S10</f>
         <v>-217.80799999999994</v>
@@ -12394,28 +12684,62 @@
         <f>T6-T10</f>
         <v>-311.93599999999998</v>
       </c>
+      <c r="AA11" s="29">
+        <f t="shared" ref="AA11" si="8">AA6-AA10</f>
+        <v>-492.90099999999984</v>
+      </c>
+      <c r="AB11" s="29">
+        <f>AB6-AB10</f>
+        <v>-915.58400000000006</v>
+      </c>
     </row>
     <row r="12" spans="1:38" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
         <v>67</v>
       </c>
+      <c r="M12" s="30">
+        <v>3.996</v>
+      </c>
+      <c r="N12" s="30">
+        <v>9.4260000000000002</v>
+      </c>
       <c r="O12" s="30">
         <v>8.3130000000000006</v>
       </c>
       <c r="P12" s="30">
         <v>24.292999999999999</v>
       </c>
+      <c r="Q12" s="30">
+        <v>6.6130000000000004</v>
+      </c>
+      <c r="R12" s="30">
+        <v>6.1260000000000003</v>
+      </c>
       <c r="S12" s="30">
         <v>6.6769999999999996</v>
       </c>
       <c r="T12" s="30">
         <v>8.2390000000000008</v>
+      </c>
+      <c r="AA12" s="30">
+        <v>11.525</v>
+      </c>
+      <c r="AB12" s="30">
+        <v>45.344999999999999</v>
       </c>
     </row>
     <row r="13" spans="1:38" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s">
         <v>76</v>
       </c>
+      <c r="M13" s="30">
+        <f t="shared" ref="M13" si="9">M11-M12</f>
+        <v>-116.26600000000001</v>
+      </c>
+      <c r="N13" s="30">
+        <f t="shared" ref="N13" si="10">N11-N12</f>
+        <v>-194.71699999999987</v>
+      </c>
       <c r="O13" s="30">
         <f>O11-O12</f>
         <v>-205.65199999999993</v>
@@ -12424,6 +12748,14 @@
         <f>P11-P12</f>
         <v>-226.56699999999995</v>
       </c>
+      <c r="Q13" s="30">
+        <f>Q11-Q12</f>
+        <v>-238.95799999999997</v>
+      </c>
+      <c r="R13" s="30">
+        <f>R11-R12</f>
+        <v>-289.75199999999995</v>
+      </c>
       <c r="S13" s="30">
         <f>S11-S12</f>
         <v>-224.48499999999993</v>
@@ -12432,28 +12764,62 @@
         <f>T11-T12</f>
         <v>-320.17499999999995</v>
       </c>
+      <c r="AA13" s="30">
+        <f>AA11-AA12</f>
+        <v>-504.42599999999982</v>
+      </c>
+      <c r="AB13" s="30">
+        <f>AB11-AB12</f>
+        <v>-960.92900000000009</v>
+      </c>
     </row>
     <row r="14" spans="1:38" x14ac:dyDescent="0.2">
       <c r="B14" s="1" t="s">
         <v>68</v>
       </c>
+      <c r="M14" s="30">
+        <v>0.64800000000000002</v>
+      </c>
+      <c r="N14" s="30">
+        <v>-15.366</v>
+      </c>
       <c r="O14" s="30">
         <v>0.89</v>
       </c>
       <c r="P14" s="30">
         <v>1.286</v>
       </c>
+      <c r="Q14" s="30">
+        <v>-14.849</v>
+      </c>
+      <c r="R14" s="30">
+        <v>1.6439999999999999</v>
+      </c>
       <c r="S14" s="30">
         <v>-2.8580000000000001</v>
       </c>
       <c r="T14" s="30">
         <v>2.5939999999999999</v>
+      </c>
+      <c r="AA14" s="30">
+        <v>-13.446999999999999</v>
+      </c>
+      <c r="AB14" s="30">
+        <v>-11.029</v>
       </c>
     </row>
     <row r="15" spans="1:38" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B15" s="2" t="s">
         <v>70</v>
       </c>
+      <c r="M15" s="29">
+        <f t="shared" ref="M15" si="11">M13-M14</f>
+        <v>-116.914</v>
+      </c>
+      <c r="N15" s="29">
+        <f t="shared" ref="N15" si="12">N13-N14</f>
+        <v>-179.35099999999989</v>
+      </c>
       <c r="O15" s="29">
         <f>O13-O14</f>
         <v>-206.54199999999992</v>
@@ -12462,6 +12828,14 @@
         <f>P13-P14</f>
         <v>-227.85299999999995</v>
       </c>
+      <c r="Q15" s="29">
+        <f t="shared" ref="Q15" si="13">Q13-Q14</f>
+        <v>-224.10899999999998</v>
+      </c>
+      <c r="R15" s="29">
+        <f>R13-R14</f>
+        <v>-291.39599999999996</v>
+      </c>
       <c r="S15" s="29">
         <f>S13-S14</f>
         <v>-221.62699999999992</v>
@@ -12470,11 +12844,27 @@
         <f>T13-T14</f>
         <v>-322.76899999999995</v>
       </c>
+      <c r="AA15" s="29">
+        <f>AA13-AA14</f>
+        <v>-490.97899999999981</v>
+      </c>
+      <c r="AB15" s="29">
+        <f>AB13-AB14</f>
+        <v>-949.90000000000009</v>
+      </c>
     </row>
     <row r="16" spans="1:38" x14ac:dyDescent="0.2">
       <c r="B16" s="1" t="s">
         <v>69</v>
       </c>
+      <c r="M16" s="28">
+        <f>M15/M17</f>
+        <v>-0.79263151132966325</v>
+      </c>
+      <c r="N16" s="28">
+        <f>N15/N17</f>
+        <v>-1.1323903265248076</v>
+      </c>
       <c r="O16" s="28">
         <f>O15/O17</f>
         <v>-1.2355912544819656</v>
@@ -12483,6 +12873,14 @@
         <f>P15/P17</f>
         <v>-1.3139765974420505</v>
       </c>
+      <c r="Q16" s="28">
+        <f>Q15/Q17</f>
+        <v>-1.2645002263567628</v>
+      </c>
+      <c r="R16" s="28">
+        <f>R15/R17</f>
+        <v>-1.628504773126946</v>
+      </c>
       <c r="S16" s="28">
         <f>S15/S17</f>
         <v>-1.2251441501410789</v>
@@ -12491,145 +12889,311 @@
         <f>T15/T17</f>
         <v>-1.7700728317826633</v>
       </c>
-    </row>
-    <row r="17" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="AA16" s="59">
+        <f>AA15/AA17</f>
+        <v>-3.3466258226346173</v>
+      </c>
+      <c r="AB16" s="59">
+        <f>AB15/AB17</f>
+        <v>-5.4535392358724044</v>
+      </c>
+    </row>
+    <row r="17" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B17" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="M17" s="59">
+        <v>147.50107499999999</v>
+      </c>
+      <c r="N17" s="59">
+        <v>158.382667</v>
+      </c>
       <c r="O17" s="28">
         <v>167.16045800000001</v>
       </c>
       <c r="P17" s="28">
         <v>173.40719799999999</v>
       </c>
+      <c r="Q17" s="59">
+        <v>177.23128500000001</v>
+      </c>
+      <c r="R17" s="28">
+        <v>178.93469200000001</v>
+      </c>
       <c r="S17" s="28">
         <v>180.89871299999999</v>
       </c>
       <c r="T17" s="28">
         <v>182.34786399999999</v>
       </c>
-    </row>
-    <row r="19" spans="2:20" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AA17" s="59">
+        <v>146.708663</v>
+      </c>
+      <c r="AB17" s="59">
+        <v>174.180465</v>
+      </c>
+    </row>
+    <row r="19" spans="2:28" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B19" s="2" t="s">
         <v>71</v>
       </c>
+      <c r="Q19" s="32">
+        <f t="shared" ref="Q19" si="14">Q4/M4-1</f>
+        <v>0.65229290419649577</v>
+      </c>
+      <c r="R19" s="32">
+        <f t="shared" ref="R19" si="15">R4/N4-1</f>
+        <v>0.53760148880658276</v>
+      </c>
       <c r="S19" s="32">
-        <f t="shared" ref="S19" si="2">S4/O4-1</f>
+        <f t="shared" ref="S19" si="16">S4/O4-1</f>
         <v>0.4836962785683776</v>
       </c>
       <c r="T19" s="32">
         <f>T4/P4-1</f>
         <v>0.41024111604933844</v>
       </c>
-    </row>
-    <row r="20" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="AB19" s="32">
+        <f>AB4/AA4-1</f>
+        <v>0.613053532344634</v>
+      </c>
+    </row>
+    <row r="20" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B20" s="1" t="s">
         <v>72</v>
+      </c>
+      <c r="N20" s="31">
+        <f t="shared" ref="N20:O20" si="17">N4/M4-1</f>
+        <v>0.22349984039074133</v>
+      </c>
+      <c r="O20" s="31">
+        <f t="shared" si="17"/>
+        <v>7.6443649765549404E-2</v>
       </c>
       <c r="P20" s="31">
         <f>P4/O4-1</f>
         <v>0.13380441636101059</v>
       </c>
+      <c r="Q20" s="31">
+        <f t="shared" ref="Q20:S20" si="18">Q4/P4-1</f>
+        <v>0.10650575320922484</v>
+      </c>
+      <c r="R20" s="31">
+        <f t="shared" si="18"/>
+        <v>0.13857244763407617</v>
+      </c>
+      <c r="S20" s="31">
+        <f t="shared" si="18"/>
+        <v>3.8705704223346515E-2</v>
+      </c>
       <c r="T20" s="31">
         <f>T4/S4-1</f>
         <v>7.7671777308385259E-2</v>
       </c>
-    </row>
-    <row r="22" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="Y20" s="60" t="s">
+        <v>1716</v>
+      </c>
+      <c r="Z20" s="60" t="s">
+        <v>1716</v>
+      </c>
+      <c r="AA20" s="60" t="s">
+        <v>1716</v>
+      </c>
+      <c r="AB20" s="60" t="s">
+        <v>1716</v>
+      </c>
+    </row>
+    <row r="22" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B22" s="1" t="s">
         <v>73</v>
       </c>
+      <c r="M22" s="31">
+        <f t="shared" ref="M22:N22" si="19">M6/M4</f>
+        <v>0.51537941241469831</v>
+      </c>
+      <c r="N22" s="31">
+        <f t="shared" ref="N22:O22" si="20">N6/N4</f>
+        <v>0.51473480632742796</v>
+      </c>
       <c r="O22" s="31">
-        <f t="shared" ref="O22:P22" si="3">O6/O4</f>
+        <f t="shared" si="20"/>
         <v>0.50561028359898841</v>
       </c>
       <c r="P22" s="31">
         <f>P6/P4</f>
         <v>0.49518859194745046</v>
       </c>
-      <c r="Q22" s="31"/>
-      <c r="R22" s="31"/>
+      <c r="Q22" s="31">
+        <f t="shared" ref="Q22:R22" si="21">Q6/Q4</f>
+        <v>0.49260581267158088</v>
+      </c>
+      <c r="R22" s="31">
+        <f t="shared" ref="R22:S22" si="22">R6/R4</f>
+        <v>0.47054265589550326</v>
+      </c>
       <c r="S22" s="31">
-        <f t="shared" ref="S22:T22" si="4">S6/S4</f>
+        <f t="shared" si="22"/>
         <v>0.48559397644177338</v>
       </c>
       <c r="T22" s="31">
         <f>T6/T4</f>
         <v>0.47202746794946543</v>
       </c>
-    </row>
-    <row r="23" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="AA22" s="31">
+        <f t="shared" ref="AA22:AB22" si="23">AA6/AA4</f>
+        <v>0.51973746946263322</v>
+      </c>
+      <c r="AB22" s="31">
+        <f>AB6/AB4</f>
+        <v>0.48937079123764576</v>
+      </c>
+    </row>
+    <row r="23" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B23" s="1" t="s">
         <v>74</v>
       </c>
+      <c r="M23" s="31">
+        <f t="shared" ref="M23:N23" si="24">M11/M4</f>
+        <v>-0.25062002058178134</v>
+      </c>
+      <c r="N23" s="31">
+        <f t="shared" ref="N23:O23" si="25">N11/N4</f>
+        <v>-0.33806674086372651</v>
+      </c>
       <c r="O23" s="31">
-        <f t="shared" ref="O23:P23" si="5">O11/O4</f>
+        <f t="shared" si="25"/>
         <v>-0.33447968433256259</v>
       </c>
       <c r="P23" s="31">
         <f>P11/P4</f>
         <v>-0.30238395290396158</v>
       </c>
-      <c r="Q23" s="31"/>
-      <c r="R23" s="31"/>
+      <c r="Q23" s="31">
+        <f t="shared" ref="Q23:R23" si="26">Q11/Q4</f>
+        <v>-0.3139050712263029</v>
+      </c>
+      <c r="R23" s="31">
+        <f t="shared" ref="R23:S23" si="27">R11/R4</f>
+        <v>-0.33655060136886167</v>
+      </c>
       <c r="S23" s="31">
-        <f t="shared" ref="S23:T23" si="6">S11/S4</f>
+        <f t="shared" si="27"/>
         <v>-0.24882020373262284</v>
       </c>
       <c r="T23" s="31">
         <f>T11/T4</f>
         <v>-0.33066696065315881</v>
       </c>
-    </row>
-    <row r="24" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="AA23" s="31">
+        <f t="shared" ref="AA23:AB23" si="28">AA11/AA4</f>
+        <v>-0.27977506788604217</v>
+      </c>
+      <c r="AB23" s="31">
+        <f>AB11/AB4</f>
+        <v>-0.32218010942914083</v>
+      </c>
+    </row>
+    <row r="24" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B24" s="1" t="s">
-        <v>68</v>
+        <v>75</v>
+      </c>
+      <c r="M24" s="31">
+        <f t="shared" ref="M24:N24" si="29">M15/M4</f>
+        <v>-0.26098680935511165</v>
+      </c>
+      <c r="N24" s="31">
+        <f t="shared" ref="N24:O24" si="30">N15/N4</f>
+        <v>-0.3272291047090804</v>
       </c>
       <c r="O24" s="31">
-        <f t="shared" ref="O24:P24" si="7">O15/O4</f>
+        <f t="shared" si="30"/>
         <v>-0.35007830667742379</v>
       </c>
       <c r="P24" s="31">
         <f>P15/P4</f>
         <v>-0.34062257542257712</v>
       </c>
-      <c r="Q24" s="31"/>
-      <c r="R24" s="31"/>
+      <c r="Q24" s="31">
+        <f t="shared" ref="Q24:R24" si="31">Q15/Q4</f>
+        <v>-0.30277798793800387</v>
+      </c>
+      <c r="R24" s="31">
+        <f t="shared" ref="R24:S24" si="32">R15/R4</f>
+        <v>-0.34577048308857727</v>
+      </c>
       <c r="S24" s="31">
-        <f t="shared" ref="S24:T24" si="8">S15/S4</f>
+        <f t="shared" si="32"/>
         <v>-0.25318296523842099</v>
       </c>
       <c r="T24" s="31">
         <f>T15/T4</f>
         <v>-0.34215045465435023</v>
       </c>
-    </row>
-    <row r="25" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="AA24" s="31">
+        <f t="shared" ref="AA24:AB24" si="33">AA15/AA4</f>
+        <v>-0.27868412329376707</v>
+      </c>
+      <c r="AB24" s="31">
+        <f>AB15/AB4</f>
+        <v>-0.33425538885207784</v>
+      </c>
+    </row>
+    <row r="25" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B25" s="1" t="s">
-        <v>75</v>
+        <v>68</v>
+      </c>
+      <c r="M25" s="31">
+        <f t="shared" ref="M25:N25" si="34">M14/M13</f>
+        <v>-5.5734264531333323E-3</v>
+      </c>
+      <c r="N25" s="31">
+        <f t="shared" ref="N25:O25" si="35">N14/N13</f>
+        <v>7.891452723696446E-2</v>
       </c>
       <c r="O25" s="31">
-        <f t="shared" ref="O25:P25" si="9">O14/O13</f>
+        <f t="shared" si="35"/>
         <v>-4.3276992200416255E-3</v>
       </c>
       <c r="P25" s="31">
         <f>P14/P13</f>
         <v>-5.6760251934306425E-3</v>
       </c>
-      <c r="Q25" s="31"/>
-      <c r="R25" s="31"/>
+      <c r="Q25" s="31">
+        <f t="shared" ref="Q25:R25" si="36">Q14/Q13</f>
+        <v>6.2140627223194043E-2</v>
+      </c>
+      <c r="R25" s="31">
+        <f t="shared" ref="R25:S25" si="37">R14/R13</f>
+        <v>-5.6738176095419536E-3</v>
+      </c>
       <c r="S25" s="31">
-        <f t="shared" ref="S25:T25" si="10">S14/S13</f>
+        <f t="shared" si="37"/>
         <v>1.2731362897298265E-2</v>
       </c>
       <c r="T25" s="31">
         <f>T14/T13</f>
         <v>-8.1018193175607101E-3</v>
       </c>
-    </row>
-    <row r="27" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="AA25" s="31">
+        <f t="shared" ref="AA25:AB25" si="38">AA14/AA13</f>
+        <v>2.6658023178821082E-2</v>
+      </c>
+      <c r="AB25" s="31">
+        <f>AB14/AB13</f>
+        <v>1.1477434857309956E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B27" s="1" t="s">
         <v>77</v>
+      </c>
+      <c r="Q27" s="31">
+        <f t="shared" ref="Q27" si="39">Q7/M7-1</f>
+        <v>0.5359453209612739</v>
+      </c>
+      <c r="R27" s="31">
+        <f t="shared" ref="R27" si="40">R7/N7-1</f>
+        <v>0.40535453492471163</v>
       </c>
       <c r="S27" s="31">
         <f>S7/O7-1</f>
@@ -12639,422 +13203,1304 @@
         <f>T7/P7-1</f>
         <v>0.54259157105030908</v>
       </c>
-    </row>
-    <row r="28" spans="2:20" s="35" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AB27" s="31">
+        <f>AB7/AA7-1</f>
+        <v>0.48755437773773536</v>
+      </c>
+    </row>
+    <row r="28" spans="2:28" s="35" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B28" s="35" t="s">
         <v>78</v>
       </c>
-      <c r="P28" s="57">
+      <c r="N28" s="42">
+        <f t="shared" ref="N28:O28" si="41">N7/M7-1</f>
+        <v>0.16248573017592149</v>
+      </c>
+      <c r="O28" s="42">
+        <f t="shared" si="41"/>
+        <v>0.10036762854409043</v>
+      </c>
+      <c r="P28" s="42">
         <f>P7/O7-1</f>
         <v>3.7070938215102878E-2</v>
       </c>
-      <c r="T28" s="57">
+      <c r="Q28" s="42">
+        <f t="shared" ref="Q28:S28" si="42">Q7/P7-1</f>
+        <v>0.15782215357458074</v>
+      </c>
+      <c r="R28" s="42">
+        <f t="shared" si="42"/>
+        <v>6.3647624946400638E-2</v>
+      </c>
+      <c r="S28" s="42">
+        <f t="shared" si="42"/>
+        <v>7.7769665261658405E-2</v>
+      </c>
+      <c r="T28" s="42">
         <f>T7/S7-1</f>
         <v>0.16221203519373617</v>
       </c>
-    </row>
-    <row r="30" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="Y28" s="60" t="s">
+        <v>1716</v>
+      </c>
+      <c r="Z28" s="60" t="s">
+        <v>1716</v>
+      </c>
+      <c r="AA28" s="60" t="s">
+        <v>1716</v>
+      </c>
+      <c r="AB28" s="60" t="s">
+        <v>1716</v>
+      </c>
+    </row>
+    <row r="30" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B30" s="34" t="s">
         <v>1710</v>
       </c>
     </row>
-    <row r="31" spans="2:20" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B31" s="1" t="s">
         <v>1711</v>
       </c>
-      <c r="O31" s="55">
+      <c r="M31" s="40">
+        <v>208000</v>
+      </c>
+      <c r="N31" s="40">
+        <v>221000</v>
+      </c>
+      <c r="O31" s="40">
         <v>235000</v>
       </c>
-      <c r="P31" s="55">
+      <c r="P31" s="40">
         <v>240000</v>
       </c>
-      <c r="S31" s="55">
+      <c r="Q31" s="40">
+        <v>250000</v>
+      </c>
+      <c r="R31" s="40">
+        <v>256000</v>
+      </c>
+      <c r="S31" s="40">
         <v>268000</v>
       </c>
-      <c r="T31" s="55">
+      <c r="T31" s="40">
         <v>275000</v>
       </c>
-    </row>
-    <row r="32" spans="2:20" s="35" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B32" s="54" t="s">
+      <c r="AA31" s="40">
+        <f>N31</f>
+        <v>221000</v>
+      </c>
+      <c r="AB31" s="40">
+        <f>R31</f>
+        <v>256000</v>
+      </c>
+    </row>
+    <row r="32" spans="2:28" s="35" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B32" s="39" t="s">
         <v>1715</v>
       </c>
-      <c r="P32" s="56"/>
-      <c r="S32" s="57">
+      <c r="P32" s="41"/>
+      <c r="Q32" s="42">
+        <f t="shared" ref="Q32" si="43">Q31/M31-1</f>
+        <v>0.20192307692307687</v>
+      </c>
+      <c r="R32" s="42">
+        <f>R31/N31-1</f>
+        <v>0.158371040723982</v>
+      </c>
+      <c r="S32" s="42">
         <f>S31/O31-1</f>
         <v>0.14042553191489371</v>
       </c>
-      <c r="T32" s="57">
+      <c r="T32" s="42">
         <f>T31/P31-1</f>
         <v>0.14583333333333326</v>
       </c>
-    </row>
-    <row r="33" spans="2:22" s="35" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B33" s="54" t="s">
+      <c r="AB32" s="42">
+        <f>AB31/AA31-1</f>
+        <v>0.158371040723982</v>
+      </c>
+    </row>
+    <row r="33" spans="2:28" s="35" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B33" s="39" t="s">
         <v>1714</v>
       </c>
-      <c r="P33" s="57">
-        <f>P31/O31-1</f>
+      <c r="N33" s="42">
+        <f t="shared" ref="N33:R33" si="44">N31/M31-1</f>
+        <v>6.25E-2</v>
+      </c>
+      <c r="O33" s="42">
+        <f t="shared" si="44"/>
+        <v>6.3348416289592757E-2</v>
+      </c>
+      <c r="P33" s="42">
+        <f t="shared" si="44"/>
         <v>2.1276595744680771E-2</v>
       </c>
-      <c r="S33" s="57"/>
-      <c r="T33" s="57">
+      <c r="Q33" s="42">
+        <f t="shared" si="44"/>
+        <v>4.1666666666666741E-2</v>
+      </c>
+      <c r="R33" s="42">
+        <f t="shared" ref="R33:S33" si="45">R31/Q31-1</f>
+        <v>2.4000000000000021E-2</v>
+      </c>
+      <c r="S33" s="42">
+        <f t="shared" si="45"/>
+        <v>4.6875E-2</v>
+      </c>
+      <c r="T33" s="42">
         <f>T31/S31-1</f>
         <v>2.6119402985074647E-2</v>
       </c>
-    </row>
-    <row r="34" spans="2:22" x14ac:dyDescent="0.2">
+      <c r="Y33" s="60" t="s">
+        <v>1716</v>
+      </c>
+      <c r="Z33" s="60" t="s">
+        <v>1716</v>
+      </c>
+      <c r="AA33" s="60" t="s">
+        <v>1716</v>
+      </c>
+      <c r="AB33" s="60" t="s">
+        <v>1716</v>
+      </c>
+    </row>
+    <row r="34" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B34" s="1" t="s">
         <v>1712</v>
       </c>
-      <c r="S34" s="55">
+      <c r="Q34" s="40">
+        <v>7381</v>
+      </c>
+      <c r="R34" s="40">
+        <v>7867</v>
+      </c>
+      <c r="S34" s="40">
         <v>8199</v>
       </c>
-      <c r="T34" s="55">
+      <c r="T34" s="40">
         <v>8510</v>
       </c>
       <c r="V34" s="30"/>
-    </row>
-    <row r="35" spans="2:22" s="35" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B35" s="54" t="s">
+      <c r="AA34" s="1">
+        <f>N34</f>
+        <v>0</v>
+      </c>
+      <c r="AB34" s="40">
+        <f>R34</f>
+        <v>7867</v>
+      </c>
+    </row>
+    <row r="35" spans="2:28" s="35" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B35" s="39" t="s">
         <v>1713</v>
       </c>
-      <c r="P35" s="58" t="e">
-        <f>P4/P34</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="S35" s="58">
+      <c r="P35" s="43"/>
+      <c r="Q35" s="43">
+        <f>Q4/Q34</f>
+        <v>0.10028126270153097</v>
+      </c>
+      <c r="R35" s="43">
+        <f>R4/R34</f>
+        <v>0.10712393542646498</v>
+      </c>
+      <c r="S35" s="43">
         <f>S4/S34</f>
         <v>0.10676460543968777</v>
       </c>
-      <c r="T35" s="58">
+      <c r="T35" s="43">
         <f>T4/T34</f>
         <v>0.1108524089306698</v>
       </c>
-    </row>
-    <row r="39" spans="2:22" x14ac:dyDescent="0.2">
+      <c r="AA35" s="43" t="e">
+        <f>AA4/AA34</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AB35" s="43">
+        <f>AB4/AB34</f>
+        <v>0.36123541375365448</v>
+      </c>
+    </row>
+    <row r="39" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B39" s="34" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="40" spans="2:22" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="2:28" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B40" s="2" t="s">
         <v>6</v>
       </c>
+      <c r="N40" s="29">
+        <v>933.88499999999999</v>
+      </c>
+      <c r="Q40" s="29">
+        <v>1497.498</v>
+      </c>
+      <c r="R40" s="29">
+        <v>1479.452</v>
+      </c>
+      <c r="S40" s="29">
+        <v>1617.0219999999999</v>
+      </c>
       <c r="T40" s="29">
         <v>798.625</v>
       </c>
-    </row>
-    <row r="41" spans="2:22" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AA40" s="29">
+        <f>N40</f>
+        <v>933.88499999999999</v>
+      </c>
+      <c r="AB40" s="29">
+        <f>R40</f>
+        <v>1479.452</v>
+      </c>
+    </row>
+    <row r="41" spans="2:28" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B41" s="2" t="s">
         <v>80</v>
       </c>
+      <c r="N41" s="29">
+        <v>2105.9059999999999</v>
+      </c>
+      <c r="Q41" s="29">
+        <v>3896.7539999999999</v>
+      </c>
+      <c r="R41" s="29">
+        <v>3878.43</v>
+      </c>
+      <c r="S41" s="29">
+        <v>3606.29</v>
+      </c>
       <c r="T41" s="29">
         <v>3593.6590000000001</v>
       </c>
-    </row>
-    <row r="42" spans="2:22" x14ac:dyDescent="0.2">
+      <c r="AA41" s="29">
+        <f t="shared" ref="AA41" si="46">N41</f>
+        <v>2105.9059999999999</v>
+      </c>
+      <c r="AB41" s="29">
+        <f>R41</f>
+        <v>3878.43</v>
+      </c>
+    </row>
+    <row r="42" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B42" s="1" t="s">
         <v>81</v>
       </c>
+      <c r="N42" s="30">
+        <v>251.167</v>
+      </c>
+      <c r="Q42" s="30">
+        <v>345.79300000000001</v>
+      </c>
+      <c r="R42" s="30">
+        <v>388.21499999999997</v>
+      </c>
+      <c r="S42" s="30">
+        <v>406.73599999999999</v>
+      </c>
       <c r="T42" s="30">
         <v>471.91500000000002</v>
       </c>
-    </row>
-    <row r="43" spans="2:22" x14ac:dyDescent="0.2">
+      <c r="AA42" s="30">
+        <f>N42</f>
+        <v>251.167</v>
+      </c>
+      <c r="AB42" s="30">
+        <f>R42</f>
+        <v>388.21499999999997</v>
+      </c>
+    </row>
+    <row r="43" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B43" s="1" t="s">
         <v>82</v>
       </c>
+      <c r="N43" s="30">
+        <v>81.376999999999995</v>
+      </c>
+      <c r="Q43" s="30">
+        <v>165.76</v>
+      </c>
+      <c r="R43" s="30">
+        <v>186.131</v>
+      </c>
+      <c r="S43" s="30">
+        <v>201.142</v>
+      </c>
       <c r="T43" s="30">
         <v>240.19200000000001</v>
       </c>
-    </row>
-    <row r="44" spans="2:22" x14ac:dyDescent="0.2">
+      <c r="AA43" s="30">
+        <f t="shared" ref="AA43" si="47">N43</f>
+        <v>81.376999999999995</v>
+      </c>
+      <c r="AB43" s="30">
+        <f t="shared" ref="AB43" si="48">R43</f>
+        <v>186.131</v>
+      </c>
+    </row>
+    <row r="44" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B44" s="1" t="s">
         <v>83</v>
+      </c>
+      <c r="N44" s="30">
+        <f>SUM(N40:N43)</f>
+        <v>3372.335</v>
+      </c>
+      <c r="Q44" s="30">
+        <f>SUM(Q40:Q43)</f>
+        <v>5905.8050000000003</v>
+      </c>
+      <c r="R44" s="30">
+        <f>SUM(R40:R43)</f>
+        <v>5932.2280000000001</v>
+      </c>
+      <c r="S44" s="30">
+        <f>SUM(S40:S43)</f>
+        <v>5831.19</v>
       </c>
       <c r="T44" s="30">
         <f>SUM(T40:T43)</f>
         <v>5104.3909999999996</v>
       </c>
-    </row>
-    <row r="45" spans="2:22" x14ac:dyDescent="0.2">
+      <c r="AA44" s="30">
+        <f t="shared" ref="AA44:AB44" si="49">SUM(AA40:AA43)</f>
+        <v>3372.335</v>
+      </c>
+      <c r="AB44" s="30">
+        <f t="shared" si="49"/>
+        <v>5932.2280000000001</v>
+      </c>
+    </row>
+    <row r="45" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B45" s="1" t="s">
         <v>84</v>
       </c>
+      <c r="N45" s="30">
+        <v>183.239</v>
+      </c>
+      <c r="Q45" s="30">
+        <v>237.24100000000001</v>
+      </c>
+      <c r="R45" s="30">
+        <v>255.316</v>
+      </c>
+      <c r="S45" s="30">
+        <v>259.00299999999999</v>
+      </c>
       <c r="T45" s="30">
         <v>264.767</v>
       </c>
-    </row>
-    <row r="46" spans="2:22" x14ac:dyDescent="0.2">
+      <c r="AA45" s="30">
+        <f t="shared" ref="AA45:AA49" si="50">N45</f>
+        <v>183.239</v>
+      </c>
+      <c r="AB45" s="30">
+        <f t="shared" ref="AB45:AB49" si="51">R45</f>
+        <v>255.316</v>
+      </c>
+    </row>
+    <row r="46" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B46" s="1" t="s">
         <v>85</v>
       </c>
+      <c r="N46" s="30">
+        <v>258.61</v>
+      </c>
+      <c r="Q46" s="30">
+        <v>248.58199999999999</v>
+      </c>
+      <c r="R46" s="30">
+        <v>234.584</v>
+      </c>
+      <c r="S46" s="30">
+        <v>225.95099999999999</v>
+      </c>
       <c r="T46" s="30">
         <v>213.464</v>
       </c>
-    </row>
-    <row r="47" spans="2:22" x14ac:dyDescent="0.2">
+      <c r="AA46" s="30">
+        <f t="shared" si="50"/>
+        <v>258.61</v>
+      </c>
+      <c r="AB46" s="30">
+        <f t="shared" si="51"/>
+        <v>234.584</v>
+      </c>
+    </row>
+    <row r="47" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B47" s="1" t="s">
         <v>86</v>
       </c>
+      <c r="N47" s="30">
+        <v>0</v>
+      </c>
+      <c r="Q47" s="30">
+        <v>0</v>
+      </c>
+      <c r="R47" s="30">
+        <v>0</v>
+      </c>
+      <c r="S47" s="30">
+        <v>0</v>
+      </c>
       <c r="T47" s="30">
         <v>750</v>
       </c>
-    </row>
-    <row r="48" spans="2:22" x14ac:dyDescent="0.2">
+      <c r="AA47" s="30">
+        <f t="shared" si="50"/>
+        <v>0</v>
+      </c>
+      <c r="AB47" s="30">
+        <f t="shared" si="51"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B48" s="1" t="s">
         <v>87</v>
+      </c>
+      <c r="N48" s="30">
+        <f>966.573+4595.394</f>
+        <v>5561.9670000000006</v>
+      </c>
+      <c r="Q48" s="30">
+        <f>1102.599+5263.051</f>
+        <v>6365.6500000000005</v>
+      </c>
+      <c r="R48" s="30">
+        <f>1050.012+5263.166</f>
+        <v>6313.1779999999999</v>
+      </c>
+      <c r="S48" s="30">
+        <f>1006.692+5286.683</f>
+        <v>6293.375</v>
       </c>
       <c r="T48" s="30">
         <f>953.522+5285.563</f>
         <v>6239.085</v>
       </c>
-    </row>
-    <row r="49" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="AA48" s="30">
+        <f t="shared" si="50"/>
+        <v>5561.9670000000006</v>
+      </c>
+      <c r="AB48" s="30">
+        <f t="shared" si="51"/>
+        <v>6313.1779999999999</v>
+      </c>
+    </row>
+    <row r="49" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B49" s="1" t="s">
         <v>88</v>
       </c>
+      <c r="N49" s="30">
+        <v>111.282</v>
+      </c>
+      <c r="Q49" s="30">
+        <v>219.56899999999999</v>
+      </c>
+      <c r="R49" s="30">
+        <v>263.29199999999997</v>
+      </c>
+      <c r="S49" s="30">
+        <v>281.28300000000002</v>
+      </c>
       <c r="T49" s="30">
         <v>297.52199999999999</v>
       </c>
-    </row>
-    <row r="50" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="AA49" s="30">
+        <f t="shared" si="50"/>
+        <v>111.282</v>
+      </c>
+      <c r="AB49" s="30">
+        <f t="shared" si="51"/>
+        <v>263.29199999999997</v>
+      </c>
+    </row>
+    <row r="50" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B50" s="1" t="s">
         <v>89</v>
+      </c>
+      <c r="N50" s="30">
+        <f>N44+SUM(N45:N49)</f>
+        <v>9487.4330000000009</v>
+      </c>
+      <c r="Q50" s="30">
+        <f>Q44+SUM(Q45:Q49)</f>
+        <v>12976.847000000002</v>
+      </c>
+      <c r="R50" s="30">
+        <f>R44+SUM(R45:R49)</f>
+        <v>12998.598</v>
+      </c>
+      <c r="S50" s="30">
+        <f>S44+SUM(S45:S49)</f>
+        <v>12890.802</v>
       </c>
       <c r="T50" s="30">
         <f>T44+SUM(T45:T49)</f>
         <v>12869.228999999999</v>
       </c>
-    </row>
-    <row r="51" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="AA50" s="30">
+        <f t="shared" ref="AA50:AB50" si="52">AA44+SUM(AA45:AA49)</f>
+        <v>9487.4330000000009</v>
+      </c>
+      <c r="AB50" s="30">
+        <f t="shared" si="52"/>
+        <v>12998.598</v>
+      </c>
+    </row>
+    <row r="51" spans="2:28" x14ac:dyDescent="0.2">
+      <c r="N51" s="30"/>
+      <c r="Q51" s="30"/>
+      <c r="S51" s="30"/>
       <c r="T51" s="30"/>
     </row>
-    <row r="52" spans="2:20" x14ac:dyDescent="0.2">
+    <row r="52" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B52" s="1" t="s">
         <v>90</v>
       </c>
+      <c r="N52" s="30">
+        <v>60.042000000000002</v>
+      </c>
+      <c r="Q52" s="30">
+        <v>76.293000000000006</v>
+      </c>
+      <c r="R52" s="30">
+        <v>93.332999999999998</v>
+      </c>
+      <c r="S52" s="30">
+        <v>93.388999999999996</v>
+      </c>
       <c r="T52" s="30">
         <v>102.039</v>
       </c>
-    </row>
-    <row r="53" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="AA52" s="30">
+        <f t="shared" ref="AA52:AA57" si="53">N52</f>
+        <v>60.042000000000002</v>
+      </c>
+      <c r="AB52" s="30">
+        <f t="shared" ref="AB52:AB55" si="54">R52</f>
+        <v>93.332999999999998</v>
+      </c>
+    </row>
+    <row r="53" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B53" s="1" t="s">
         <v>91</v>
       </c>
+      <c r="N53" s="30">
+        <v>252.89500000000001</v>
+      </c>
+      <c r="Q53" s="30">
+        <v>368.863</v>
+      </c>
+      <c r="R53" s="30">
+        <v>417.50299999999999</v>
+      </c>
+      <c r="S53" s="30">
+        <v>433.66800000000001</v>
+      </c>
       <c r="T53" s="30">
         <v>504.81</v>
       </c>
-    </row>
-    <row r="54" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="AA53" s="30">
+        <f t="shared" si="53"/>
+        <v>252.89500000000001</v>
+      </c>
+      <c r="AB53" s="30">
+        <f t="shared" si="54"/>
+        <v>417.50299999999999</v>
+      </c>
+    </row>
+    <row r="54" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B54" s="1" t="s">
         <v>92</v>
       </c>
+      <c r="N54" s="30">
+        <v>87.031000000000006</v>
+      </c>
+      <c r="Q54" s="30">
+        <v>121.337</v>
+      </c>
+      <c r="R54" s="30">
+        <v>140.38900000000001</v>
+      </c>
+      <c r="S54" s="30">
+        <v>139.67099999999999</v>
+      </c>
       <c r="T54" s="30">
         <v>137.72800000000001</v>
       </c>
-    </row>
-    <row r="55" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="AA54" s="30">
+        <f t="shared" si="53"/>
+        <v>87.031000000000006</v>
+      </c>
+      <c r="AB54" s="30">
+        <f t="shared" si="54"/>
+        <v>140.38900000000001</v>
+      </c>
+    </row>
+    <row r="55" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B55" s="1" t="s">
         <v>93</v>
       </c>
+      <c r="N55" s="30">
+        <v>48.338000000000001</v>
+      </c>
+      <c r="Q55" s="30">
+        <v>50.76</v>
+      </c>
+      <c r="R55" s="30">
+        <v>52.325000000000003</v>
+      </c>
+      <c r="S55" s="30">
+        <v>53.094000000000001</v>
+      </c>
       <c r="T55" s="30">
         <v>50.743000000000002</v>
       </c>
-    </row>
-    <row r="56" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="AA55" s="30">
+        <f t="shared" si="53"/>
+        <v>48.338000000000001</v>
+      </c>
+      <c r="AB55" s="30">
+        <f t="shared" si="54"/>
+        <v>52.325000000000003</v>
+      </c>
+    </row>
+    <row r="56" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B56" s="1" t="s">
         <v>94</v>
+      </c>
+      <c r="N56" s="30">
+        <f>SUM(N52:N55)</f>
+        <v>448.30600000000004</v>
+      </c>
+      <c r="Q56" s="30">
+        <v>617.07299999999998</v>
+      </c>
+      <c r="R56" s="30">
+        <f>SUM(R52:R55)</f>
+        <v>703.55000000000007</v>
+      </c>
+      <c r="S56" s="30">
+        <f>SUM(S52:S55)</f>
+        <v>719.82200000000012</v>
       </c>
       <c r="T56" s="30">
         <f>SUM(T52:T55)</f>
         <v>795.32</v>
       </c>
-    </row>
-    <row r="57" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="AA56" s="30">
+        <f t="shared" ref="AA56:AB56" si="55">SUM(AA52:AA55)</f>
+        <v>448.30600000000004</v>
+      </c>
+      <c r="AB56" s="30">
+        <f t="shared" si="55"/>
+        <v>703.55000000000007</v>
+      </c>
+    </row>
+    <row r="57" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B57" s="1" t="s">
         <v>93</v>
       </c>
+      <c r="N57" s="30">
+        <v>229.905</v>
+      </c>
+      <c r="Q57" s="30">
+        <v>223.03299999999999</v>
+      </c>
+      <c r="R57" s="30">
+        <v>211.25299999999999</v>
+      </c>
+      <c r="S57" s="30">
+        <v>201.35400000000001</v>
+      </c>
       <c r="T57" s="30">
         <v>189.06800000000001</v>
       </c>
-    </row>
-    <row r="58" spans="2:20" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AA57" s="30">
+        <f t="shared" si="53"/>
+        <v>229.905</v>
+      </c>
+      <c r="AB57" s="30">
+        <f t="shared" ref="AB57" si="56">R57</f>
+        <v>211.25299999999999</v>
+      </c>
+    </row>
+    <row r="58" spans="2:28" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B58" s="2" t="s">
         <v>95</v>
       </c>
+      <c r="N58" s="29">
+        <v>17.856000000000002</v>
+      </c>
+      <c r="Q58" s="29">
+        <v>20.254000000000001</v>
+      </c>
+      <c r="R58" s="29">
+        <v>25.132000000000001</v>
+      </c>
+      <c r="S58" s="29">
+        <v>22.053000000000001</v>
+      </c>
       <c r="T58" s="29">
         <v>18.934999999999999</v>
       </c>
-    </row>
-    <row r="59" spans="2:20" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AA58" s="29">
+        <f t="shared" ref="AA58" si="57">N58</f>
+        <v>17.856000000000002</v>
+      </c>
+      <c r="AB58" s="29">
+        <f>R58</f>
+        <v>25.132000000000001</v>
+      </c>
+    </row>
+    <row r="59" spans="2:28" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B59" s="2" t="s">
         <v>96</v>
       </c>
+      <c r="N59" s="29">
+        <v>302.06799999999998</v>
+      </c>
+      <c r="Q59" s="29">
+        <v>985.54700000000003</v>
+      </c>
+      <c r="R59" s="29">
+        <v>985.90700000000004</v>
+      </c>
+      <c r="S59" s="29">
+        <v>986.24300000000005</v>
+      </c>
       <c r="T59" s="29">
         <v>986.61900000000003</v>
       </c>
-    </row>
-    <row r="60" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="AA59" s="29">
+        <f t="shared" ref="AA59:AA60" si="58">N59</f>
+        <v>302.06799999999998</v>
+      </c>
+      <c r="AB59" s="29">
+        <f t="shared" ref="AB59:AB60" si="59">R59</f>
+        <v>985.90700000000004</v>
+      </c>
+    </row>
+    <row r="60" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B60" s="1" t="s">
         <v>97</v>
       </c>
+      <c r="N60" s="30">
+        <v>36.633000000000003</v>
+      </c>
+      <c r="Q60" s="30">
+        <v>49.191000000000003</v>
+      </c>
+      <c r="R60" s="30">
+        <v>41.29</v>
+      </c>
+      <c r="S60" s="30">
+        <v>43.896999999999998</v>
+      </c>
       <c r="T60" s="30">
         <v>37.292000000000002</v>
       </c>
-    </row>
-    <row r="61" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="AA60" s="30">
+        <f t="shared" si="58"/>
+        <v>36.633000000000003</v>
+      </c>
+      <c r="AB60" s="30">
+        <f t="shared" si="59"/>
+        <v>41.29</v>
+      </c>
+    </row>
+    <row r="61" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B61" s="1" t="s">
         <v>98</v>
+      </c>
+      <c r="N61" s="30">
+        <f>SUM(N57:N60)+N56</f>
+        <v>1034.768</v>
+      </c>
+      <c r="Q61" s="30">
+        <f>SUM(Q57:Q60)+Q56</f>
+        <v>1895.098</v>
+      </c>
+      <c r="R61" s="30">
+        <f>SUM(R57:R60)+R56</f>
+        <v>1967.1320000000001</v>
+      </c>
+      <c r="S61" s="30">
+        <f>SUM(S57:S60)+S56</f>
+        <v>1973.3690000000001</v>
       </c>
       <c r="T61" s="30">
         <f>SUM(T57:T60)+T56</f>
         <v>2027.2339999999999</v>
       </c>
-    </row>
-    <row r="62" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="AA61" s="30">
+        <f>SUM(AA57:AA60)+AA56</f>
+        <v>1034.768</v>
+      </c>
+      <c r="AB61" s="30">
+        <f>SUM(AB57:AB60)+AB56</f>
+        <v>1967.1320000000001</v>
+      </c>
+    </row>
+    <row r="62" spans="2:28" x14ac:dyDescent="0.2">
       <c r="T62" s="30"/>
     </row>
-    <row r="63" spans="2:20" x14ac:dyDescent="0.2">
+    <row r="63" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B63" s="1" t="s">
         <v>99</v>
       </c>
+      <c r="N63" s="30">
+        <v>8452.6650000000009</v>
+      </c>
+      <c r="Q63" s="30">
+        <v>11081.749</v>
+      </c>
+      <c r="R63" s="30">
+        <v>11031.466</v>
+      </c>
+      <c r="S63" s="30">
+        <v>10917.433000000001</v>
+      </c>
       <c r="T63" s="30">
         <v>10841.995000000001</v>
       </c>
-    </row>
-    <row r="64" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="AA63" s="30">
+        <f>N63</f>
+        <v>8452.6650000000009</v>
+      </c>
+      <c r="AB63" s="30">
+        <f>R63</f>
+        <v>11031.466</v>
+      </c>
+    </row>
+    <row r="64" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B64" s="1" t="s">
         <v>100</v>
+      </c>
+      <c r="N64" s="30">
+        <f>N63+N61</f>
+        <v>9487.4330000000009</v>
+      </c>
+      <c r="Q64" s="30">
+        <f>Q63+Q61</f>
+        <v>12976.847</v>
+      </c>
+      <c r="R64" s="30">
+        <f>R63+R61</f>
+        <v>12998.598</v>
+      </c>
+      <c r="S64" s="30">
+        <f>S63+S61</f>
+        <v>12890.802000000001</v>
       </c>
       <c r="T64" s="30">
         <f>T63+T61</f>
         <v>12869.229000000001</v>
       </c>
-    </row>
-    <row r="66" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="AA64" s="30">
+        <f>AA63+AA61</f>
+        <v>9487.4330000000009</v>
+      </c>
+      <c r="AB64" s="30">
+        <f>AB63+AB61</f>
+        <v>12998.598</v>
+      </c>
+    </row>
+    <row r="66" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B66" s="1" t="s">
         <v>101</v>
+      </c>
+      <c r="N66" s="30">
+        <f t="shared" ref="N66" si="60">N50-N61</f>
+        <v>8452.6650000000009</v>
+      </c>
+      <c r="Q66" s="30">
+        <f t="shared" ref="Q66:R66" si="61">Q50-Q61</f>
+        <v>11081.749000000002</v>
+      </c>
+      <c r="R66" s="30">
+        <f t="shared" si="61"/>
+        <v>11031.466</v>
+      </c>
+      <c r="S66" s="30">
+        <f t="shared" ref="S66" si="62">S50-S61</f>
+        <v>10917.432999999999</v>
       </c>
       <c r="T66" s="30">
         <f>T50-T61</f>
         <v>10841.994999999999</v>
       </c>
-    </row>
-    <row r="67" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="AA66" s="30">
+        <f>AA50-AA61</f>
+        <v>8452.6650000000009</v>
+      </c>
+      <c r="AB66" s="30">
+        <f>AB50-AB61</f>
+        <v>11031.466</v>
+      </c>
+    </row>
+    <row r="67" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B67" s="1" t="s">
         <v>102</v>
+      </c>
+      <c r="N67" s="1">
+        <f t="shared" ref="N67" si="63">N66/N17</f>
+        <v>53.368623979541908</v>
+      </c>
+      <c r="Q67" s="1">
+        <f t="shared" ref="Q67" si="64">Q66/Q17</f>
+        <v>62.527047637215972</v>
+      </c>
+      <c r="R67" s="1">
+        <f t="shared" ref="R67" si="65">R66/R17</f>
+        <v>61.650794916840383</v>
+      </c>
+      <c r="S67" s="1">
+        <f t="shared" ref="S67" si="66">S66/S17</f>
+        <v>60.351081657501894</v>
       </c>
       <c r="T67" s="1">
         <f>T66/T17</f>
         <v>59.457757070299436</v>
       </c>
-    </row>
-    <row r="69" spans="2:20" s="35" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AA67" s="1">
+        <f>AA66/AA17</f>
+        <v>57.615309329074869</v>
+      </c>
+      <c r="AB67" s="1">
+        <f>AB66/AB17</f>
+        <v>63.333543173168131</v>
+      </c>
+    </row>
+    <row r="69" spans="2:28" s="35" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B69" s="35" t="s">
         <v>6</v>
+      </c>
+      <c r="N69" s="36">
+        <f>N40+N41</f>
+        <v>3039.7910000000002</v>
+      </c>
+      <c r="Q69" s="36">
+        <f t="shared" ref="Q69:R69" si="67">Q40+Q41</f>
+        <v>5394.2520000000004</v>
+      </c>
+      <c r="R69" s="36">
+        <f>R40+R41</f>
+        <v>5357.8819999999996</v>
+      </c>
+      <c r="S69" s="36">
+        <f>S40+S41</f>
+        <v>5223.3119999999999</v>
       </c>
       <c r="T69" s="36">
         <f>T40+T41</f>
         <v>4392.2839999999997</v>
       </c>
-    </row>
-    <row r="70" spans="2:20" s="35" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AA69" s="36">
+        <f>N69</f>
+        <v>3039.7910000000002</v>
+      </c>
+      <c r="AB69" s="36">
+        <f>R69</f>
+        <v>5357.8819999999996</v>
+      </c>
+    </row>
+    <row r="70" spans="2:28" s="35" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B70" s="35" t="s">
         <v>7</v>
+      </c>
+      <c r="N70" s="36">
+        <f>N58+N59</f>
+        <v>319.92399999999998</v>
+      </c>
+      <c r="Q70" s="36">
+        <f t="shared" ref="Q70:R70" si="68">Q58+Q59</f>
+        <v>1005.801</v>
+      </c>
+      <c r="R70" s="36">
+        <f>R58+R59</f>
+        <v>1011.039</v>
+      </c>
+      <c r="S70" s="36">
+        <f>S58+S59</f>
+        <v>1008.296</v>
       </c>
       <c r="T70" s="36">
         <f>T58+T59</f>
         <v>1005.554</v>
       </c>
-    </row>
-    <row r="71" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="AA70" s="36">
+        <f>N70</f>
+        <v>319.92399999999998</v>
+      </c>
+      <c r="AB70" s="36">
+        <f>R70</f>
+        <v>1011.039</v>
+      </c>
+    </row>
+    <row r="71" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B71" s="1" t="s">
         <v>8</v>
+      </c>
+      <c r="N71" s="30">
+        <f t="shared" ref="N71" si="69">N69-N70</f>
+        <v>2719.8670000000002</v>
+      </c>
+      <c r="Q71" s="30">
+        <f t="shared" ref="Q71" si="70">Q69-Q70</f>
+        <v>4388.451</v>
+      </c>
+      <c r="R71" s="30">
+        <f t="shared" ref="R71" si="71">R69-R70</f>
+        <v>4346.8429999999998</v>
+      </c>
+      <c r="S71" s="30">
+        <f t="shared" ref="S71" si="72">S69-S70</f>
+        <v>4215.0159999999996</v>
       </c>
       <c r="T71" s="30">
         <f>T69-T70</f>
         <v>3386.7299999999996</v>
       </c>
-    </row>
-    <row r="73" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="AA71" s="30">
+        <f>AA69-AA70</f>
+        <v>2719.8670000000002</v>
+      </c>
+      <c r="AB71" s="30">
+        <f>AB69-AB70</f>
+        <v>4346.8429999999998</v>
+      </c>
+    </row>
+    <row r="73" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B73" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="M73" s="1">
+        <v>247.09</v>
+      </c>
+      <c r="N73" s="59">
+        <v>338.5</v>
+      </c>
+      <c r="O73" s="1">
+        <v>340.76</v>
+      </c>
       <c r="P73" s="1">
         <v>394.16</v>
       </c>
+      <c r="Q73" s="1">
+        <v>319.05</v>
+      </c>
       <c r="R73" s="1">
         <v>263.33999999999997</v>
       </c>
+      <c r="S73" s="1">
+        <v>164.81</v>
+      </c>
       <c r="T73" s="1">
         <v>83.81</v>
       </c>
-    </row>
-    <row r="74" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="AA73" s="59">
+        <f>N73</f>
+        <v>338.5</v>
+      </c>
+      <c r="AB73" s="1">
+        <f>R73</f>
+        <v>263.33999999999997</v>
+      </c>
+    </row>
+    <row r="74" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B74" s="1" t="s">
         <v>5</v>
+      </c>
+      <c r="M74" s="30">
+        <f>M73*M17</f>
+        <v>36446.040621749999</v>
+      </c>
+      <c r="N74" s="30">
+        <f>N73*N17</f>
+        <v>53612.532779499998</v>
+      </c>
+      <c r="O74" s="30">
+        <f>O73*O17</f>
+        <v>56961.597668080001</v>
       </c>
       <c r="P74" s="30">
         <f>P73*P17</f>
         <v>68350.181163679998</v>
       </c>
-      <c r="Q74" s="30"/>
-      <c r="R74" s="30"/>
-      <c r="S74" s="30"/>
+      <c r="Q74" s="30">
+        <f>Q73*Q17</f>
+        <v>56545.641479250007</v>
+      </c>
+      <c r="R74" s="30">
+        <f>R73*R17</f>
+        <v>47120.661791279999</v>
+      </c>
+      <c r="S74" s="30">
+        <f>S73*S17</f>
+        <v>29813.916889529999</v>
+      </c>
       <c r="T74" s="30">
         <f>T73*T17</f>
         <v>15282.57448184</v>
       </c>
-    </row>
-    <row r="75" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="AA74" s="30">
+        <f>AA73*AA17</f>
+        <v>49660.8824255</v>
+      </c>
+      <c r="AB74" s="30">
+        <f>AB73*AB17</f>
+        <v>45868.683653099994</v>
+      </c>
+    </row>
+    <row r="75" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B75" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="N75" s="30">
+        <f t="shared" ref="N75" si="73">N74-N71</f>
+        <v>50892.665779499999</v>
+      </c>
       <c r="P75" s="30"/>
       <c r="Q75" s="30"/>
-      <c r="R75" s="30"/>
-      <c r="S75" s="30"/>
+      <c r="R75" s="30">
+        <f t="shared" ref="R75" si="74">R74-R71</f>
+        <v>42773.818791279999</v>
+      </c>
+      <c r="S75" s="30">
+        <f t="shared" ref="S75" si="75">S74-S71</f>
+        <v>25598.900889529999</v>
+      </c>
       <c r="T75" s="30">
         <f>T74-T71</f>
         <v>11895.84448184</v>
       </c>
-    </row>
-    <row r="77" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="AA75" s="30">
+        <f t="shared" ref="AA75" si="76">AA74-AA71</f>
+        <v>46941.015425500002</v>
+      </c>
+      <c r="AB75" s="30">
+        <f t="shared" ref="AB75" si="77">AB74-AB71</f>
+        <v>41521.840653099993</v>
+      </c>
+    </row>
+    <row r="77" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B77" s="1" t="s">
         <v>103</v>
+      </c>
+      <c r="N77" s="37">
+        <f>N73/N67</f>
+        <v>6.3426780523657325</v>
+      </c>
+      <c r="Q77" s="37">
+        <f t="shared" ref="Q77:R77" si="78">Q73/Q67</f>
+        <v>5.1025917911739382</v>
+      </c>
+      <c r="R77" s="37">
+        <f>R73/R67</f>
+        <v>4.2714777701603754</v>
+      </c>
+      <c r="S77" s="37">
+        <f>S73/S67</f>
+        <v>2.730854120151688</v>
       </c>
       <c r="T77" s="37">
         <f>T73/T67</f>
         <v>1.4095721757702342</v>
       </c>
-    </row>
-    <row r="78" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="AA77" s="37">
+        <f>AA73/AA67</f>
+        <v>5.8751745663054189</v>
+      </c>
+      <c r="AB77" s="37">
+        <f>AB73/AB67</f>
+        <v>4.1579862235082805</v>
+      </c>
+    </row>
+    <row r="78" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B78" s="1" t="s">
         <v>105</v>
       </c>
+      <c r="N78" s="37">
+        <f t="shared" ref="N78" si="79">N74/SUM(K4:N4)</f>
+        <v>53.82465574780209</v>
+      </c>
+      <c r="Q78" s="37">
+        <f t="shared" ref="Q78" si="80">Q74/SUM(N4:Q4)</f>
+        <v>22.199267614739412</v>
+      </c>
+      <c r="R78" s="37">
+        <f t="shared" ref="R78:S78" si="81">R74/SUM(O4:R4)</f>
+        <v>16.581045510065838</v>
+      </c>
+      <c r="S78" s="37">
+        <f t="shared" si="81"/>
+        <v>9.5336989696036145</v>
+      </c>
       <c r="T78" s="37">
-        <f>T74/T4</f>
-        <v>16.200254074122757</v>
-      </c>
-    </row>
-    <row r="79" spans="2:20" x14ac:dyDescent="0.2">
+        <f>T74/SUM(Q4:T4)</f>
+        <v>4.4927117390362339</v>
+      </c>
+      <c r="AA78" s="37">
+        <f>AA74/AA4</f>
+        <v>28.187966248546921</v>
+      </c>
+      <c r="AB78" s="37">
+        <f>AB74/AB4</f>
+        <v>16.140493410464138</v>
+      </c>
+    </row>
+    <row r="79" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B79" s="1" t="s">
         <v>104</v>
       </c>
+      <c r="N79" s="37">
+        <f t="shared" ref="N79" si="82">N73/SUM(K16:N16)</f>
+        <v>-175.84216103089744</v>
+      </c>
+      <c r="Q79" s="37">
+        <f t="shared" ref="Q79" si="83">Q73/SUM(N16:Q16)</f>
+        <v>-64.500694009685063</v>
+      </c>
+      <c r="R79" s="37">
+        <f t="shared" ref="R79:S79" si="84">R73/SUM(O16:R16)</f>
+        <v>-48.385204422553002</v>
+      </c>
+      <c r="S79" s="37">
+        <f t="shared" si="84"/>
+        <v>-30.339872026893296</v>
+      </c>
       <c r="T79" s="37">
-        <f>T73/T16</f>
-        <v>-47.348334201363834</v>
+        <f>T73/SUM(Q16:T16)</f>
+        <v>-14.233498713981406</v>
+      </c>
+      <c r="AA79" s="37">
+        <f>AA73/AA16</f>
+        <v>-101.14665276009771</v>
+      </c>
+      <c r="AB79" s="37">
+        <f>AB73/AB16</f>
+        <v>-48.287907835666907</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="T1" r:id="rId1" xr:uid="{A7A5BBDF-38B5-4BC3-94A5-ED2C969CF757}"/>
     <hyperlink ref="S1" r:id="rId2" xr:uid="{A6D6F957-F960-45B2-92A0-A41F2E0A1924}"/>
+    <hyperlink ref="R1" r:id="rId3" xr:uid="{A293EABB-9A75-4B29-8553-BB352A36DBB6}"/>
+    <hyperlink ref="AB1" r:id="rId4" xr:uid="{442A1034-B338-4801-AF1E-61BA7E0E77AC}"/>
+    <hyperlink ref="Q1" r:id="rId5" xr:uid="{BA74861F-598C-41FE-BE22-C6AA1B8966A6}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="256" orientation="portrait" horizontalDpi="203" verticalDpi="203" r:id="rId3"/>
+  <pageSetup paperSize="256" orientation="portrait" horizontalDpi="203" verticalDpi="203" r:id="rId6"/>
+  <ignoredErrors>
+    <ignoredError sqref="AA44:AB44 AA56:AB56" formula="1"/>
+    <ignoredError sqref="N78:P78 S78:T78 Q78:R78" formulaRange="1"/>
+  </ignoredErrors>
+  <drawing r:id="rId7"/>
 </worksheet>
 </file>
 
@@ -13062,13 +14508,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33C88468-B575-4B07-B1E2-1E3BE5EA25D5}">
   <dimension ref="A1:G1596"/>
   <sheetViews>
-    <sheetView topLeftCell="A1552" workbookViewId="0">
-      <selection activeCell="E1596" sqref="E1596"/>
+    <sheetView topLeftCell="A1016" workbookViewId="0">
+      <selection activeCell="F1046" sqref="F1046"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="1"/>
+    <col min="1" max="1" width="23.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="6" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="16384" width="9.140625" style="1"/>

</xml_diff>

<commit_message>
Add FY18, FY19 data to $TWLO
</commit_message>
<xml_diff>
--- a/$TWLO.xlsx
+++ b/$TWLO.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\me\Documents\Google Drive\Stocks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{590D7F15-5151-4503-80F3-7D1678541F9A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55736C3F-E0B2-464E-9D68-47C84D3995CD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{1EC168B4-1311-4642-A238-D70265844B27}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" activeTab="1" xr2:uid="{1EC168B4-1311-4642-A238-D70265844B27}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -26,8 +26,66 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>me</author>
+  </authors>
+  <commentList>
+    <comment ref="F47" authorId="0" shapeId="0" xr:uid="{55D6C87D-C1A4-4EF5-9464-1503FD9AE294}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>me:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Restricted Cash</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J47" authorId="0" shapeId="0" xr:uid="{BCD95C05-2508-4246-A1FE-77A2158ED6BC}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>me:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Restricted Cash</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1742" uniqueCount="1717">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1744" uniqueCount="1717">
   <si>
     <t>$TWLO</t>
   </si>
@@ -5189,7 +5247,7 @@
     <numFmt numFmtId="165" formatCode="0.0\x"/>
     <numFmt numFmtId="166" formatCode="#,##0.0000"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -5259,6 +5317,19 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -5466,6 +5537,19 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -5491,19 +5575,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -11267,7 +11338,7 @@
     <xdr:to>
       <xdr:col>20</xdr:col>
       <xdr:colOff>19050</xdr:colOff>
-      <xdr:row>84</xdr:row>
+      <xdr:row>85</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -11317,7 +11388,7 @@
     <xdr:to>
       <xdr:col>28</xdr:col>
       <xdr:colOff>19050</xdr:colOff>
-      <xdr:row>84</xdr:row>
+      <xdr:row>85</xdr:row>
       <xdr:rowOff>66675</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -11659,8 +11730,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF09F688-7B08-4E67-BE87-6887CCA7D948}">
   <dimension ref="B2:R35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="W2" sqref="S2:W2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M41" sqref="M41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -11673,20 +11744,20 @@
         <v>0</v>
       </c>
       <c r="F2"/>
-      <c r="G2" s="61" t="s">
+      <c r="G2" s="46" t="s">
         <v>1716</v>
       </c>
-      <c r="H2" s="61"/>
-      <c r="I2" s="61"/>
-      <c r="J2" s="61"/>
-      <c r="K2" s="61"/>
-      <c r="L2" s="61"/>
-      <c r="M2" s="61"/>
-      <c r="N2" s="61"/>
-      <c r="O2" s="61"/>
-      <c r="P2" s="61"/>
-      <c r="Q2" s="61"/>
-      <c r="R2" s="61"/>
+      <c r="H2" s="46"/>
+      <c r="I2" s="46"/>
+      <c r="J2" s="46"/>
+      <c r="K2" s="46"/>
+      <c r="L2" s="46"/>
+      <c r="M2" s="46"/>
+      <c r="N2" s="46"/>
+      <c r="O2" s="46"/>
+      <c r="P2" s="46"/>
+      <c r="Q2" s="46"/>
+      <c r="R2" s="46"/>
     </row>
     <row r="3" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B3" s="2" t="s">
@@ -11694,24 +11765,24 @@
       </c>
     </row>
     <row r="5" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B5" s="46" t="s">
+      <c r="B5" s="53" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="47"/>
-      <c r="D5" s="48"/>
-      <c r="G5" s="46" t="s">
+      <c r="C5" s="54"/>
+      <c r="D5" s="55"/>
+      <c r="G5" s="53" t="s">
         <v>24</v>
       </c>
-      <c r="H5" s="47"/>
-      <c r="I5" s="47"/>
-      <c r="J5" s="47"/>
-      <c r="K5" s="47"/>
-      <c r="L5" s="47"/>
-      <c r="M5" s="47"/>
-      <c r="N5" s="47"/>
-      <c r="O5" s="47"/>
-      <c r="P5" s="47"/>
-      <c r="Q5" s="48"/>
+      <c r="H5" s="54"/>
+      <c r="I5" s="54"/>
+      <c r="J5" s="54"/>
+      <c r="K5" s="54"/>
+      <c r="L5" s="54"/>
+      <c r="M5" s="54"/>
+      <c r="N5" s="54"/>
+      <c r="O5" s="54"/>
+      <c r="P5" s="54"/>
+      <c r="Q5" s="55"/>
     </row>
     <row r="6" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B6" s="5" t="s">
@@ -11783,7 +11854,7 @@
         <v>6</v>
       </c>
       <c r="C9" s="18">
-        <f>'Financial Model'!T69</f>
+        <f>'Financial Model'!T70</f>
         <v>4392.2839999999997</v>
       </c>
       <c r="D9" s="16" t="str">
@@ -11807,7 +11878,7 @@
         <v>7</v>
       </c>
       <c r="C10" s="18">
-        <f>'Financial Model'!T70</f>
+        <f>'Financial Model'!T71</f>
         <v>1005.554</v>
       </c>
       <c r="D10" s="16" t="str">
@@ -11898,11 +11969,11 @@
       <c r="Q14" s="9"/>
     </row>
     <row r="15" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B15" s="46" t="s">
+      <c r="B15" s="53" t="s">
         <v>10</v>
       </c>
-      <c r="C15" s="47"/>
-      <c r="D15" s="48"/>
+      <c r="C15" s="54"/>
+      <c r="D15" s="55"/>
       <c r="G15" s="20"/>
       <c r="H15" s="8"/>
       <c r="I15" s="8"/>
@@ -11919,10 +11990,10 @@
       <c r="B16" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="C16" s="55" t="s">
+      <c r="C16" s="49" t="s">
         <v>22</v>
       </c>
-      <c r="D16" s="56"/>
+      <c r="D16" s="50"/>
       <c r="G16" s="20"/>
       <c r="H16" s="8"/>
       <c r="I16" s="8"/>
@@ -11939,8 +12010,8 @@
       <c r="B17" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C17" s="57"/>
-      <c r="D17" s="58"/>
+      <c r="C17" s="47"/>
+      <c r="D17" s="48"/>
       <c r="G17" s="20"/>
       <c r="H17" s="8"/>
       <c r="I17" s="8"/>
@@ -11957,10 +12028,10 @@
       <c r="B18" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="C18" s="55" t="s">
+      <c r="C18" s="49" t="s">
         <v>23</v>
       </c>
-      <c r="D18" s="56"/>
+      <c r="D18" s="50"/>
       <c r="G18" s="20"/>
       <c r="H18" s="8"/>
       <c r="I18" s="8"/>
@@ -11977,8 +12048,8 @@
       <c r="B19" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="C19" s="59"/>
-      <c r="D19" s="60"/>
+      <c r="C19" s="51"/>
+      <c r="D19" s="52"/>
       <c r="G19" s="20"/>
       <c r="H19" s="8"/>
       <c r="I19" s="8"/>
@@ -12018,11 +12089,11 @@
       <c r="Q21" s="9"/>
     </row>
     <row r="22" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B22" s="46" t="s">
+      <c r="B22" s="53" t="s">
         <v>15</v>
       </c>
-      <c r="C22" s="47"/>
-      <c r="D22" s="48"/>
+      <c r="C22" s="54"/>
+      <c r="D22" s="55"/>
       <c r="G22" s="20"/>
       <c r="H22" s="8"/>
       <c r="I22" s="8"/>
@@ -12039,10 +12110,10 @@
       <c r="B23" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="C23" s="55" t="s">
+      <c r="C23" s="49" t="s">
         <v>21</v>
       </c>
-      <c r="D23" s="56"/>
+      <c r="D23" s="50"/>
       <c r="G23" s="20"/>
       <c r="H23" s="8"/>
       <c r="I23" s="8"/>
@@ -12059,10 +12130,10 @@
       <c r="B24" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="C24" s="55">
+      <c r="C24" s="49">
         <v>2008</v>
       </c>
-      <c r="D24" s="56"/>
+      <c r="D24" s="50"/>
       <c r="G24" s="20"/>
       <c r="H24" s="8"/>
       <c r="I24" s="8"/>
@@ -12077,8 +12148,8 @@
     </row>
     <row r="25" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B25" s="13"/>
-      <c r="C25" s="55"/>
-      <c r="D25" s="56"/>
+      <c r="C25" s="49"/>
+      <c r="D25" s="50"/>
       <c r="G25" s="20"/>
       <c r="H25" s="8"/>
       <c r="I25" s="8"/>
@@ -12093,8 +12164,8 @@
     </row>
     <row r="26" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B26" s="13"/>
-      <c r="C26" s="55"/>
-      <c r="D26" s="56"/>
+      <c r="C26" s="49"/>
+      <c r="D26" s="50"/>
       <c r="G26" s="20"/>
       <c r="H26" s="8"/>
       <c r="I26" s="8"/>
@@ -12109,8 +12180,8 @@
     </row>
     <row r="27" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B27" s="13"/>
-      <c r="C27" s="55"/>
-      <c r="D27" s="56"/>
+      <c r="C27" s="49"/>
+      <c r="D27" s="50"/>
       <c r="G27" s="20"/>
       <c r="H27" s="8"/>
       <c r="I27" s="8"/>
@@ -12150,10 +12221,10 @@
       <c r="B29" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="C29" s="53" t="s">
+      <c r="C29" s="60" t="s">
         <v>20</v>
       </c>
-      <c r="D29" s="54"/>
+      <c r="D29" s="61"/>
       <c r="G29" s="21"/>
       <c r="H29" s="11"/>
       <c r="I29" s="11"/>
@@ -12167,52 +12238,44 @@
       <c r="Q29" s="12"/>
     </row>
     <row r="32" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B32" s="46" t="s">
+      <c r="B32" s="53" t="s">
         <v>106</v>
       </c>
-      <c r="C32" s="47"/>
-      <c r="D32" s="48"/>
+      <c r="C32" s="54"/>
+      <c r="D32" s="55"/>
     </row>
     <row r="33" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B33" s="13" t="s">
         <v>103</v>
       </c>
-      <c r="C33" s="49">
-        <f>'Financial Model'!T77</f>
+      <c r="C33" s="56">
+        <f>'Financial Model'!T78</f>
         <v>1.4095721757702342</v>
       </c>
-      <c r="D33" s="50"/>
+      <c r="D33" s="57"/>
     </row>
     <row r="34" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B34" s="13" t="s">
         <v>105</v>
       </c>
-      <c r="C34" s="49">
-        <f>'Financial Model'!T78</f>
+      <c r="C34" s="56">
+        <f>'Financial Model'!T79</f>
         <v>4.4927117390362339</v>
       </c>
-      <c r="D34" s="50"/>
+      <c r="D34" s="57"/>
     </row>
     <row r="35" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B35" s="14" t="s">
         <v>104</v>
       </c>
-      <c r="C35" s="51">
-        <f>'Financial Model'!T79</f>
+      <c r="C35" s="58">
+        <f>'Financial Model'!T80</f>
         <v>-14.233498713981406</v>
       </c>
-      <c r="D35" s="52"/>
+      <c r="D35" s="59"/>
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="G2:R2"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="G5:Q5"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="B15:D15"/>
-    <mergeCell ref="C16:D16"/>
     <mergeCell ref="B32:D32"/>
     <mergeCell ref="C33:D33"/>
     <mergeCell ref="C34:D34"/>
@@ -12224,6 +12287,14 @@
     <mergeCell ref="C25:D25"/>
     <mergeCell ref="C24:D24"/>
     <mergeCell ref="C23:D23"/>
+    <mergeCell ref="G2:R2"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="G5:Q5"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="B15:D15"/>
+    <mergeCell ref="C16:D16"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C29:D29" r:id="rId1" display="Link" xr:uid="{14045B38-8430-46EA-8F9C-1AE5F20888F1}"/>
@@ -12235,14 +12306,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12572CDF-F7C9-4E5D-B993-E2CE69E727D4}">
-  <dimension ref="A1:AL79"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12572CDF-F7C9-4E5D-B993-E2CE69E727D4}">
+  <dimension ref="A1:AL80"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="W24" sqref="W24"/>
+      <selection pane="bottomRight" activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -12276,7 +12347,7 @@
       <c r="I1" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="J1" s="22" t="s">
+      <c r="J1" s="27" t="s">
         <v>32</v>
       </c>
       <c r="K1" s="22" t="s">
@@ -12315,10 +12386,10 @@
       <c r="V1" s="22" t="s">
         <v>44</v>
       </c>
-      <c r="Y1" s="22" t="s">
+      <c r="Y1" s="27" t="s">
         <v>45</v>
       </c>
-      <c r="Z1" s="22" t="s">
+      <c r="Z1" s="27" t="s">
         <v>46</v>
       </c>
       <c r="AA1" s="22" t="s">
@@ -12360,6 +12431,12 @@
     </row>
     <row r="2" spans="1:38" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="23"/>
+      <c r="F2" s="26">
+        <v>43465</v>
+      </c>
+      <c r="J2" s="26">
+        <v>43830</v>
+      </c>
       <c r="M2" s="26">
         <v>44104</v>
       </c>
@@ -12384,6 +12461,12 @@
       <c r="T2" s="26">
         <v>44742</v>
       </c>
+      <c r="Y2" s="26">
+        <v>43465</v>
+      </c>
+      <c r="Z2" s="26">
+        <v>43830</v>
+      </c>
       <c r="AA2" s="26">
         <v>44196</v>
       </c>
@@ -12393,6 +12476,9 @@
     </row>
     <row r="3" spans="1:38" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="23"/>
+      <c r="J3" s="25">
+        <v>38384</v>
+      </c>
       <c r="Q3" s="25">
         <v>46661</v>
       </c>
@@ -12404,6 +12490,9 @@
       </c>
       <c r="T3" s="25">
         <v>38200</v>
+      </c>
+      <c r="Z3" s="25">
+        <v>38384</v>
       </c>
       <c r="AB3" s="25">
         <v>39845</v>
@@ -12413,6 +12502,12 @@
       <c r="B4" s="2" t="s">
         <v>59</v>
       </c>
+      <c r="F4" s="29">
+        <v>204.30199999999999</v>
+      </c>
+      <c r="J4" s="29">
+        <v>331.22399999999999</v>
+      </c>
       <c r="M4" s="29">
         <v>447.96899999999999</v>
       </c>
@@ -12436,6 +12531,14 @@
       </c>
       <c r="T4" s="29">
         <v>943.35400000000004</v>
+      </c>
+      <c r="U4" s="29"/>
+      <c r="V4" s="29"/>
+      <c r="Y4" s="29">
+        <v>650.06700000000001</v>
+      </c>
+      <c r="Z4" s="29">
+        <v>1134.4680000000001</v>
       </c>
       <c r="AA4" s="29">
         <v>1761.7760000000001</v>
@@ -12448,6 +12551,12 @@
       <c r="B5" s="1" t="s">
         <v>60</v>
       </c>
+      <c r="F5" s="30">
+        <v>96.287999999999997</v>
+      </c>
+      <c r="J5" s="30">
+        <v>156.53399999999999</v>
+      </c>
       <c r="M5" s="30">
         <v>217.095</v>
       </c>
@@ -12471,6 +12580,12 @@
       </c>
       <c r="T5" s="30">
         <v>498.065</v>
+      </c>
+      <c r="Y5" s="30">
+        <v>300.84100000000001</v>
+      </c>
+      <c r="Z5" s="30">
+        <v>525.55100000000004</v>
       </c>
       <c r="AA5" s="30">
         <v>846.11500000000001</v>
@@ -12483,37 +12598,53 @@
       <c r="B6" s="2" t="s">
         <v>61</v>
       </c>
+      <c r="F6" s="29">
+        <f t="shared" ref="F6" si="0">F4-F5</f>
+        <v>108.014</v>
+      </c>
+      <c r="J6" s="29">
+        <f t="shared" ref="J6" si="1">J4-J5</f>
+        <v>174.69</v>
+      </c>
       <c r="M6" s="29">
-        <f t="shared" ref="M6" si="0">M4-M5</f>
+        <f t="shared" ref="M6" si="2">M4-M5</f>
         <v>230.874</v>
       </c>
       <c r="N6" s="29">
-        <f t="shared" ref="N6:T6" si="1">N4-N5</f>
+        <f t="shared" ref="N6:T6" si="3">N4-N5</f>
         <v>282.12100000000004</v>
       </c>
       <c r="O6" s="29">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>298.30400000000003</v>
       </c>
       <c r="P6" s="29">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>331.24700000000001</v>
       </c>
       <c r="Q6" s="29">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>364.61500000000007</v>
       </c>
       <c r="R6" s="29">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>396.54700000000003</v>
       </c>
       <c r="S6" s="29">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>425.07100000000008</v>
       </c>
       <c r="T6" s="29">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>445.28900000000004</v>
+      </c>
+      <c r="Y6" s="29">
+        <f t="shared" ref="Y6:Z6" si="4">Y4-Y5</f>
+        <v>349.226</v>
+      </c>
+      <c r="Z6" s="29">
+        <f t="shared" si="4"/>
+        <v>608.91700000000003</v>
       </c>
       <c r="AA6" s="29">
         <f>AA4-AA5</f>
@@ -12528,6 +12659,12 @@
       <c r="B7" s="1" t="s">
         <v>62</v>
       </c>
+      <c r="F7" s="30">
+        <v>51.631</v>
+      </c>
+      <c r="J7" s="30">
+        <v>110.236</v>
+      </c>
       <c r="M7" s="30">
         <v>136.65199999999999</v>
       </c>
@@ -12551,6 +12688,12 @@
       </c>
       <c r="T7" s="30">
         <v>279.64100000000002</v>
+      </c>
+      <c r="Y7" s="30">
+        <v>171.358</v>
+      </c>
+      <c r="Z7" s="30">
+        <v>391.35500000000002</v>
       </c>
       <c r="AA7" s="30">
         <v>530.548</v>
@@ -12563,6 +12706,12 @@
       <c r="B8" s="1" t="s">
         <v>63</v>
       </c>
+      <c r="F8" s="30">
+        <v>59.034999999999997</v>
+      </c>
+      <c r="J8" s="30">
+        <v>106.39400000000001</v>
+      </c>
       <c r="M8" s="30">
         <v>140.875</v>
       </c>
@@ -12586,6 +12735,12 @@
       </c>
       <c r="T8" s="30">
         <v>334.95800000000003</v>
+      </c>
+      <c r="Y8" s="30">
+        <v>175.55500000000001</v>
+      </c>
+      <c r="Z8" s="30">
+        <v>369.07900000000001</v>
       </c>
       <c r="AA8" s="30">
         <v>567.40700000000004</v>
@@ -12598,6 +12753,12 @@
       <c r="B9" s="1" t="s">
         <v>64</v>
       </c>
+      <c r="F9" s="30">
+        <v>41.335000000000001</v>
+      </c>
+      <c r="J9" s="30">
+        <v>51.859000000000002</v>
+      </c>
       <c r="M9" s="30">
         <v>65.617000000000004</v>
       </c>
@@ -12621,6 +12782,12 @@
       </c>
       <c r="T9" s="30">
         <v>142.626</v>
+      </c>
+      <c r="Y9" s="30">
+        <v>117.548</v>
+      </c>
+      <c r="Z9" s="30">
+        <v>218.268</v>
       </c>
       <c r="AA9" s="30">
         <v>310.60700000000003</v>
@@ -12633,16 +12800,24 @@
       <c r="B10" s="1" t="s">
         <v>65</v>
       </c>
+      <c r="F10" s="30">
+        <f t="shared" ref="F10" si="5">SUM(F7:F9)</f>
+        <v>152.001</v>
+      </c>
+      <c r="J10" s="30">
+        <f t="shared" ref="J10" si="6">SUM(J7:J9)</f>
+        <v>268.48899999999998</v>
+      </c>
       <c r="M10" s="30">
-        <f t="shared" ref="M10:O10" si="2">SUM(M7:M9)</f>
+        <f t="shared" ref="M10:O10" si="7">SUM(M7:M9)</f>
         <v>343.14400000000001</v>
       </c>
       <c r="N10" s="30">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>467.41199999999992</v>
       </c>
       <c r="O10" s="30">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>495.64299999999997</v>
       </c>
       <c r="P10" s="30">
@@ -12650,11 +12825,11 @@
         <v>533.52099999999996</v>
       </c>
       <c r="Q10" s="30">
-        <f t="shared" ref="Q10" si="3">SUM(Q7:Q9)</f>
+        <f t="shared" ref="Q10" si="8">SUM(Q7:Q9)</f>
         <v>596.96</v>
       </c>
       <c r="R10" s="30">
-        <f t="shared" ref="R10" si="4">SUM(R7:R9)</f>
+        <f t="shared" ref="R10" si="9">SUM(R7:R9)</f>
         <v>680.173</v>
       </c>
       <c r="S10" s="30">
@@ -12665,8 +12840,16 @@
         <f>SUM(T7:T9)</f>
         <v>757.22500000000002</v>
       </c>
+      <c r="Y10" s="30">
+        <f t="shared" ref="Y10:AA10" si="10">SUM(Y7:Y9)</f>
+        <v>464.46100000000001</v>
+      </c>
+      <c r="Z10" s="30">
+        <f t="shared" si="10"/>
+        <v>978.702</v>
+      </c>
       <c r="AA10" s="30">
-        <f t="shared" ref="AA10" si="5">SUM(AA7:AA9)</f>
+        <f t="shared" si="10"/>
         <v>1408.5619999999999</v>
       </c>
       <c r="AB10" s="30">
@@ -12678,16 +12861,24 @@
       <c r="B11" s="2" t="s">
         <v>66</v>
       </c>
+      <c r="F11" s="29">
+        <f t="shared" ref="F11" si="11">F6-F10</f>
+        <v>-43.987000000000009</v>
+      </c>
+      <c r="J11" s="29">
+        <f t="shared" ref="J11" si="12">J6-J10</f>
+        <v>-93.798999999999978</v>
+      </c>
       <c r="M11" s="29">
-        <f t="shared" ref="M11:O11" si="6">M6-M10</f>
+        <f t="shared" ref="M11:O11" si="13">M6-M10</f>
         <v>-112.27000000000001</v>
       </c>
       <c r="N11" s="29">
-        <f t="shared" si="6"/>
+        <f t="shared" si="13"/>
         <v>-185.29099999999988</v>
       </c>
       <c r="O11" s="29">
-        <f t="shared" si="6"/>
+        <f t="shared" si="13"/>
         <v>-197.33899999999994</v>
       </c>
       <c r="P11" s="29">
@@ -12695,11 +12886,11 @@
         <v>-202.27399999999994</v>
       </c>
       <c r="Q11" s="29">
-        <f t="shared" ref="Q11" si="7">Q6-Q10</f>
+        <f t="shared" ref="Q11" si="14">Q6-Q10</f>
         <v>-232.34499999999997</v>
       </c>
       <c r="R11" s="29">
-        <f t="shared" ref="R11" si="8">R6-R10</f>
+        <f t="shared" ref="R11" si="15">R6-R10</f>
         <v>-283.62599999999998</v>
       </c>
       <c r="S11" s="29">
@@ -12710,8 +12901,16 @@
         <f>T6-T10</f>
         <v>-311.93599999999998</v>
       </c>
+      <c r="Y11" s="29">
+        <f t="shared" ref="Y11:AA11" si="16">Y6-Y10</f>
+        <v>-115.23500000000001</v>
+      </c>
+      <c r="Z11" s="29">
+        <f t="shared" si="16"/>
+        <v>-369.78499999999997</v>
+      </c>
       <c r="AA11" s="29">
-        <f t="shared" ref="AA11" si="9">AA6-AA10</f>
+        <f t="shared" si="16"/>
         <v>-492.90099999999984</v>
       </c>
       <c r="AB11" s="29">
@@ -12723,6 +12922,12 @@
       <c r="B12" s="1" t="s">
         <v>67</v>
       </c>
+      <c r="F12" s="30">
+        <v>2.7509999999999999</v>
+      </c>
+      <c r="J12" s="30">
+        <v>-4.7080000000000002</v>
+      </c>
       <c r="M12" s="30">
         <v>3.996</v>
       </c>
@@ -12746,6 +12951,12 @@
       </c>
       <c r="T12" s="30">
         <v>8.2390000000000008</v>
+      </c>
+      <c r="Y12" s="30">
+        <v>5.923</v>
+      </c>
+      <c r="Z12" s="30">
+        <v>-7.569</v>
       </c>
       <c r="AA12" s="30">
         <v>11.525</v>
@@ -12758,37 +12969,53 @@
       <c r="B13" s="1" t="s">
         <v>76</v>
       </c>
+      <c r="F13" s="30">
+        <f t="shared" ref="F13" si="17">F11-F12</f>
+        <v>-46.738000000000007</v>
+      </c>
+      <c r="J13" s="30">
+        <f t="shared" ref="J13" si="18">J11-J12</f>
+        <v>-89.09099999999998</v>
+      </c>
       <c r="M13" s="30">
-        <f t="shared" ref="M13" si="10">M11-M12</f>
+        <f t="shared" ref="M13" si="19">M11-M12</f>
         <v>-116.26600000000001</v>
       </c>
       <c r="N13" s="30">
-        <f t="shared" ref="N13" si="11">N11-N12</f>
+        <f t="shared" ref="N13" si="20">N11-N12</f>
         <v>-194.71699999999987</v>
       </c>
       <c r="O13" s="30">
-        <f t="shared" ref="O13:T13" si="12">O11-O12</f>
+        <f t="shared" ref="O13:T13" si="21">O11-O12</f>
         <v>-205.65199999999993</v>
       </c>
       <c r="P13" s="30">
-        <f t="shared" si="12"/>
+        <f t="shared" si="21"/>
         <v>-226.56699999999995</v>
       </c>
       <c r="Q13" s="30">
-        <f t="shared" si="12"/>
+        <f t="shared" si="21"/>
         <v>-238.95799999999997</v>
       </c>
       <c r="R13" s="30">
-        <f t="shared" si="12"/>
+        <f t="shared" si="21"/>
         <v>-289.75199999999995</v>
       </c>
       <c r="S13" s="30">
-        <f t="shared" si="12"/>
+        <f t="shared" si="21"/>
         <v>-224.48499999999993</v>
       </c>
       <c r="T13" s="30">
-        <f t="shared" si="12"/>
+        <f t="shared" si="21"/>
         <v>-320.17499999999995</v>
+      </c>
+      <c r="Y13" s="30">
+        <f t="shared" ref="Y13:Z13" si="22">Y11-Y12</f>
+        <v>-121.15800000000002</v>
+      </c>
+      <c r="Z13" s="30">
+        <f t="shared" si="22"/>
+        <v>-362.21599999999995</v>
       </c>
       <c r="AA13" s="30">
         <f>AA11-AA12</f>
@@ -12803,6 +13030,12 @@
       <c r="B14" s="1" t="s">
         <v>68</v>
       </c>
+      <c r="F14" s="30">
+        <v>0.42</v>
+      </c>
+      <c r="J14" s="30">
+        <v>1.1559999999999999</v>
+      </c>
       <c r="M14" s="30">
         <v>0.64800000000000002</v>
       </c>
@@ -12826,6 +13059,12 @@
       </c>
       <c r="T14" s="30">
         <v>2.5939999999999999</v>
+      </c>
+      <c r="Y14" s="30">
+        <v>0.79100000000000004</v>
+      </c>
+      <c r="Z14" s="30">
+        <v>-55.152999999999999</v>
       </c>
       <c r="AA14" s="30">
         <v>-13.446999999999999</v>
@@ -12838,12 +13077,20 @@
       <c r="B15" s="2" t="s">
         <v>70</v>
       </c>
+      <c r="F15" s="29">
+        <f t="shared" ref="F15" si="23">F13-F14</f>
+        <v>-47.158000000000008</v>
+      </c>
+      <c r="J15" s="29">
+        <f t="shared" ref="J15" si="24">J13-J14</f>
+        <v>-90.246999999999986</v>
+      </c>
       <c r="M15" s="29">
-        <f t="shared" ref="M15" si="13">M13-M14</f>
+        <f t="shared" ref="M15" si="25">M13-M14</f>
         <v>-116.914</v>
       </c>
       <c r="N15" s="29">
-        <f t="shared" ref="N15" si="14">N13-N14</f>
+        <f t="shared" ref="N15" si="26">N13-N14</f>
         <v>-179.35099999999989</v>
       </c>
       <c r="O15" s="29">
@@ -12855,7 +13102,7 @@
         <v>-227.85299999999995</v>
       </c>
       <c r="Q15" s="29">
-        <f t="shared" ref="Q15" si="15">Q13-Q14</f>
+        <f t="shared" ref="Q15" si="27">Q13-Q14</f>
         <v>-224.10899999999998</v>
       </c>
       <c r="R15" s="29">
@@ -12870,6 +13117,14 @@
         <f>T13-T14</f>
         <v>-322.76899999999995</v>
       </c>
+      <c r="Y15" s="29">
+        <f t="shared" ref="Y15:Z15" si="28">Y13-Y14</f>
+        <v>-121.94900000000001</v>
+      </c>
+      <c r="Z15" s="29">
+        <f t="shared" si="28"/>
+        <v>-307.06299999999993</v>
+      </c>
       <c r="AA15" s="29">
         <f>AA13-AA14</f>
         <v>-490.97899999999981</v>
@@ -12883,37 +13138,53 @@
       <c r="B16" s="1" t="s">
         <v>69</v>
       </c>
+      <c r="F16" s="28">
+        <f t="shared" ref="F16" si="29">F15/F17</f>
+        <v>-0.47434110160515558</v>
+      </c>
+      <c r="J16" s="28">
+        <f t="shared" ref="J16" si="30">J15/J17</f>
+        <v>-0.65525253589708876</v>
+      </c>
       <c r="M16" s="28">
-        <f t="shared" ref="M16:T16" si="16">M15/M17</f>
+        <f t="shared" ref="M16:T16" si="31">M15/M17</f>
         <v>-0.79263151132966325</v>
       </c>
       <c r="N16" s="28">
-        <f t="shared" si="16"/>
+        <f t="shared" si="31"/>
         <v>-1.1323903265248076</v>
       </c>
       <c r="O16" s="28">
-        <f t="shared" si="16"/>
+        <f t="shared" si="31"/>
         <v>-1.2355912544819656</v>
       </c>
       <c r="P16" s="28">
-        <f t="shared" si="16"/>
+        <f t="shared" si="31"/>
         <v>-1.3139765974420505</v>
       </c>
       <c r="Q16" s="28">
-        <f t="shared" si="16"/>
+        <f t="shared" si="31"/>
         <v>-1.2645002263567628</v>
       </c>
       <c r="R16" s="28">
-        <f t="shared" si="16"/>
+        <f t="shared" si="31"/>
         <v>-1.628504773126946</v>
       </c>
       <c r="S16" s="28">
-        <f t="shared" si="16"/>
+        <f t="shared" si="31"/>
         <v>-1.2251441501410789</v>
       </c>
       <c r="T16" s="28">
-        <f t="shared" si="16"/>
+        <f t="shared" si="31"/>
         <v>-1.7700728317826633</v>
+      </c>
+      <c r="Y16" s="44">
+        <f t="shared" ref="Y16:Z16" si="32">Y15/Y17</f>
+        <v>-1.2555191431999431</v>
+      </c>
+      <c r="Z16" s="44">
+        <f t="shared" si="32"/>
+        <v>-2.3605151435337697</v>
       </c>
       <c r="AA16" s="44">
         <f>AA15/AA17</f>
@@ -12928,6 +13199,15 @@
       <c r="B17" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="F17" s="44">
+        <v>99.417907999999997</v>
+      </c>
+      <c r="G17" s="44"/>
+      <c r="H17" s="44"/>
+      <c r="I17" s="44"/>
+      <c r="J17" s="44">
+        <v>137.728578</v>
+      </c>
       <c r="M17" s="44">
         <v>147.50107499999999</v>
       </c>
@@ -12951,6 +13231,12 @@
       </c>
       <c r="T17" s="28">
         <v>182.34786399999999</v>
+      </c>
+      <c r="Y17" s="44">
+        <v>97.130339000000006</v>
+      </c>
+      <c r="Z17" s="44">
+        <v>130.083046</v>
       </c>
       <c r="AA17" s="44">
         <v>146.708663</v>
@@ -12963,22 +13249,38 @@
       <c r="B19" s="2" t="s">
         <v>71</v>
       </c>
+      <c r="J19" s="32">
+        <f t="shared" ref="J19" si="33">J4/F4-1</f>
+        <v>0.62124697751368063</v>
+      </c>
+      <c r="N19" s="32">
+        <f t="shared" ref="N19" si="34">N4/J4-1</f>
+        <v>0.65474120232833388</v>
+      </c>
       <c r="Q19" s="32">
-        <f t="shared" ref="Q19" si="17">Q4/M4-1</f>
+        <f t="shared" ref="Q19" si="35">Q4/M4-1</f>
         <v>0.65229290419649577</v>
       </c>
       <c r="R19" s="32">
-        <f t="shared" ref="R19" si="18">R4/N4-1</f>
+        <f t="shared" ref="R19" si="36">R4/N4-1</f>
         <v>0.53760148880658276</v>
       </c>
       <c r="S19" s="32">
-        <f t="shared" ref="S19" si="19">S4/O4-1</f>
+        <f t="shared" ref="S19" si="37">S4/O4-1</f>
         <v>0.4836962785683776</v>
       </c>
       <c r="T19" s="32">
         <f>T4/P4-1</f>
         <v>0.41024111604933844</v>
       </c>
+      <c r="Z19" s="32">
+        <f t="shared" ref="Z19:AB19" si="38">Z4/Y4-1</f>
+        <v>0.74515549935622039</v>
+      </c>
+      <c r="AA19" s="32">
+        <f t="shared" si="38"/>
+        <v>0.55295345483521796</v>
+      </c>
       <c r="AB19" s="32">
         <f>AB4/AA4-1</f>
         <v>0.613053532344634</v>
@@ -12989,11 +13291,11 @@
         <v>72</v>
       </c>
       <c r="N20" s="31">
-        <f t="shared" ref="N20:O20" si="20">N4/M4-1</f>
+        <f t="shared" ref="N20:O20" si="39">N4/M4-1</f>
         <v>0.22349984039074133</v>
       </c>
       <c r="O20" s="31">
-        <f t="shared" si="20"/>
+        <f t="shared" si="39"/>
         <v>7.6443649765549404E-2</v>
       </c>
       <c r="P20" s="31">
@@ -13001,15 +13303,15 @@
         <v>0.13380441636101059</v>
       </c>
       <c r="Q20" s="31">
-        <f t="shared" ref="Q20:S20" si="21">Q4/P4-1</f>
+        <f t="shared" ref="Q20:S20" si="40">Q4/P4-1</f>
         <v>0.10650575320922484</v>
       </c>
       <c r="R20" s="31">
-        <f t="shared" si="21"/>
+        <f t="shared" si="40"/>
         <v>0.13857244763407617</v>
       </c>
       <c r="S20" s="31">
-        <f t="shared" si="21"/>
+        <f t="shared" si="40"/>
         <v>3.8705704223346515E-2</v>
       </c>
       <c r="T20" s="31">
@@ -13033,16 +13335,24 @@
       <c r="B22" s="1" t="s">
         <v>73</v>
       </c>
+      <c r="F22" s="31">
+        <f t="shared" ref="F22" si="41">F6/F4</f>
+        <v>0.52869771221035522</v>
+      </c>
+      <c r="J22" s="31">
+        <f t="shared" ref="J22" si="42">J6/J4</f>
+        <v>0.52740743424389536</v>
+      </c>
       <c r="M22" s="31">
-        <f t="shared" ref="M22" si="22">M6/M4</f>
+        <f t="shared" ref="M22" si="43">M6/M4</f>
         <v>0.51537941241469831</v>
       </c>
       <c r="N22" s="31">
-        <f t="shared" ref="N22:O22" si="23">N6/N4</f>
+        <f t="shared" ref="N22:O22" si="44">N6/N4</f>
         <v>0.51473480632742796</v>
       </c>
       <c r="O22" s="31">
-        <f t="shared" si="23"/>
+        <f t="shared" si="44"/>
         <v>0.50561028359898841</v>
       </c>
       <c r="P22" s="31">
@@ -13050,23 +13360,31 @@
         <v>0.49518859194745046</v>
       </c>
       <c r="Q22" s="31">
-        <f t="shared" ref="Q22" si="24">Q6/Q4</f>
+        <f t="shared" ref="Q22" si="45">Q6/Q4</f>
         <v>0.49260581267158088</v>
       </c>
       <c r="R22" s="31">
-        <f t="shared" ref="R22:S22" si="25">R6/R4</f>
+        <f t="shared" ref="R22:S22" si="46">R6/R4</f>
         <v>0.47054265589550326</v>
       </c>
       <c r="S22" s="31">
-        <f t="shared" si="25"/>
+        <f t="shared" si="46"/>
         <v>0.48559397644177338</v>
       </c>
       <c r="T22" s="31">
         <f>T6/T4</f>
         <v>0.47202746794946543</v>
       </c>
+      <c r="Y22" s="31">
+        <f t="shared" ref="Y22:AA22" si="47">Y6/Y4</f>
+        <v>0.53721539472085189</v>
+      </c>
+      <c r="Z22" s="31">
+        <f t="shared" si="47"/>
+        <v>0.53674233208869704</v>
+      </c>
       <c r="AA22" s="31">
-        <f t="shared" ref="AA22" si="26">AA6/AA4</f>
+        <f t="shared" si="47"/>
         <v>0.51973746946263322</v>
       </c>
       <c r="AB22" s="31">
@@ -13078,16 +13396,24 @@
       <c r="B23" s="1" t="s">
         <v>74</v>
       </c>
+      <c r="F23" s="31">
+        <f t="shared" ref="F23" si="48">F11/F4</f>
+        <v>-0.21530381494062717</v>
+      </c>
+      <c r="J23" s="31">
+        <f t="shared" ref="J23" si="49">J11/J4</f>
+        <v>-0.28318902011931496</v>
+      </c>
       <c r="M23" s="31">
-        <f t="shared" ref="M23" si="27">M11/M4</f>
+        <f t="shared" ref="M23" si="50">M11/M4</f>
         <v>-0.25062002058178134</v>
       </c>
       <c r="N23" s="31">
-        <f t="shared" ref="N23:O23" si="28">N11/N4</f>
+        <f t="shared" ref="N23:O23" si="51">N11/N4</f>
         <v>-0.33806674086372651</v>
       </c>
       <c r="O23" s="31">
-        <f t="shared" si="28"/>
+        <f t="shared" si="51"/>
         <v>-0.33447968433256259</v>
       </c>
       <c r="P23" s="31">
@@ -13095,23 +13421,31 @@
         <v>-0.30238395290396158</v>
       </c>
       <c r="Q23" s="31">
-        <f t="shared" ref="Q23" si="29">Q11/Q4</f>
+        <f t="shared" ref="Q23" si="52">Q11/Q4</f>
         <v>-0.3139050712263029</v>
       </c>
       <c r="R23" s="31">
-        <f t="shared" ref="R23:S23" si="30">R11/R4</f>
+        <f t="shared" ref="R23:S23" si="53">R11/R4</f>
         <v>-0.33655060136886167</v>
       </c>
       <c r="S23" s="31">
-        <f t="shared" si="30"/>
+        <f t="shared" si="53"/>
         <v>-0.24882020373262284</v>
       </c>
       <c r="T23" s="31">
         <f>T11/T4</f>
         <v>-0.33066696065315881</v>
       </c>
+      <c r="Y23" s="31">
+        <f t="shared" ref="Y23:AA23" si="54">Y11/Y4</f>
+        <v>-0.17726634331538135</v>
+      </c>
+      <c r="Z23" s="31">
+        <f t="shared" si="54"/>
+        <v>-0.32595454433267396</v>
+      </c>
       <c r="AA23" s="31">
-        <f t="shared" ref="AA23" si="31">AA11/AA4</f>
+        <f t="shared" si="54"/>
         <v>-0.27977506788604217</v>
       </c>
       <c r="AB23" s="31">
@@ -13123,16 +13457,24 @@
       <c r="B24" s="1" t="s">
         <v>75</v>
       </c>
+      <c r="F24" s="31">
+        <f t="shared" ref="F24" si="55">F15/F4</f>
+        <v>-0.23082495521336066</v>
+      </c>
+      <c r="J24" s="31">
+        <f t="shared" ref="J24" si="56">J15/J4</f>
+        <v>-0.27246515952950268</v>
+      </c>
       <c r="M24" s="31">
-        <f t="shared" ref="M24" si="32">M15/M4</f>
+        <f t="shared" ref="M24" si="57">M15/M4</f>
         <v>-0.26098680935511165</v>
       </c>
       <c r="N24" s="31">
-        <f t="shared" ref="N24:O24" si="33">N15/N4</f>
+        <f t="shared" ref="N24:O24" si="58">N15/N4</f>
         <v>-0.3272291047090804</v>
       </c>
       <c r="O24" s="31">
-        <f t="shared" si="33"/>
+        <f t="shared" si="58"/>
         <v>-0.35007830667742379</v>
       </c>
       <c r="P24" s="31">
@@ -13140,23 +13482,31 @@
         <v>-0.34062257542257712</v>
       </c>
       <c r="Q24" s="31">
-        <f t="shared" ref="Q24" si="34">Q15/Q4</f>
+        <f t="shared" ref="Q24" si="59">Q15/Q4</f>
         <v>-0.30277798793800387</v>
       </c>
       <c r="R24" s="31">
-        <f t="shared" ref="R24:S24" si="35">R15/R4</f>
+        <f t="shared" ref="R24:S24" si="60">R15/R4</f>
         <v>-0.34577048308857727</v>
       </c>
       <c r="S24" s="31">
-        <f t="shared" si="35"/>
+        <f t="shared" si="60"/>
         <v>-0.25318296523842099</v>
       </c>
       <c r="T24" s="31">
         <f>T15/T4</f>
         <v>-0.34215045465435023</v>
       </c>
+      <c r="Y24" s="31">
+        <f t="shared" ref="Y24:AA24" si="61">Y15/Y4</f>
+        <v>-0.18759450948902193</v>
+      </c>
+      <c r="Z24" s="31">
+        <f t="shared" si="61"/>
+        <v>-0.27066695578896882</v>
+      </c>
       <c r="AA24" s="31">
-        <f t="shared" ref="AA24" si="36">AA15/AA4</f>
+        <f t="shared" si="61"/>
         <v>-0.27868412329376707</v>
       </c>
       <c r="AB24" s="31">
@@ -13168,16 +13518,24 @@
       <c r="B25" s="1" t="s">
         <v>68</v>
       </c>
+      <c r="F25" s="31">
+        <f t="shared" ref="F25" si="62">F14/F13</f>
+        <v>-8.9862638538234403E-3</v>
+      </c>
+      <c r="J25" s="31">
+        <f t="shared" ref="J25" si="63">J14/J13</f>
+        <v>-1.297549696377861E-2</v>
+      </c>
       <c r="M25" s="31">
-        <f t="shared" ref="M25" si="37">M14/M13</f>
+        <f t="shared" ref="M25" si="64">M14/M13</f>
         <v>-5.5734264531333323E-3</v>
       </c>
       <c r="N25" s="31">
-        <f t="shared" ref="N25:O25" si="38">N14/N13</f>
+        <f t="shared" ref="N25:O25" si="65">N14/N13</f>
         <v>7.891452723696446E-2</v>
       </c>
       <c r="O25" s="31">
-        <f t="shared" si="38"/>
+        <f t="shared" si="65"/>
         <v>-4.3276992200416255E-3</v>
       </c>
       <c r="P25" s="31">
@@ -13185,23 +13543,31 @@
         <v>-5.6760251934306425E-3</v>
       </c>
       <c r="Q25" s="31">
-        <f t="shared" ref="Q25" si="39">Q14/Q13</f>
+        <f t="shared" ref="Q25" si="66">Q14/Q13</f>
         <v>6.2140627223194043E-2</v>
       </c>
       <c r="R25" s="31">
-        <f t="shared" ref="R25:S25" si="40">R14/R13</f>
+        <f t="shared" ref="R25:S25" si="67">R14/R13</f>
         <v>-5.6738176095419536E-3</v>
       </c>
       <c r="S25" s="31">
-        <f t="shared" si="40"/>
+        <f t="shared" si="67"/>
         <v>1.2731362897298265E-2</v>
       </c>
       <c r="T25" s="31">
         <f>T14/T13</f>
         <v>-8.1018193175607101E-3</v>
       </c>
+      <c r="Y25" s="31">
+        <f t="shared" ref="Y25:AA25" si="68">Y14/Y13</f>
+        <v>-6.5286650489443532E-3</v>
+      </c>
+      <c r="Z25" s="31">
+        <f t="shared" si="68"/>
+        <v>0.15226549903924733</v>
+      </c>
       <c r="AA25" s="31">
-        <f t="shared" ref="AA25" si="41">AA14/AA13</f>
+        <f t="shared" si="68"/>
         <v>2.6658023178821082E-2</v>
       </c>
       <c r="AB25" s="31">
@@ -13213,12 +13579,20 @@
       <c r="B27" s="1" t="s">
         <v>77</v>
       </c>
+      <c r="J27" s="31">
+        <f t="shared" ref="J27" si="69">J7/F7-1</f>
+        <v>1.1350738897174177</v>
+      </c>
+      <c r="N27" s="31">
+        <f t="shared" ref="N27" si="70">N7/J7-1</f>
+        <v>0.44105373925033553</v>
+      </c>
       <c r="Q27" s="31">
-        <f t="shared" ref="Q27" si="42">Q7/M7-1</f>
+        <f t="shared" ref="Q27" si="71">Q7/M7-1</f>
         <v>0.5359453209612739</v>
       </c>
       <c r="R27" s="31">
-        <f t="shared" ref="R27" si="43">R7/N7-1</f>
+        <f t="shared" ref="R27" si="72">R7/N7-1</f>
         <v>0.40535453492471163</v>
       </c>
       <c r="S27" s="31">
@@ -13229,6 +13603,17 @@
         <f>T7/P7-1</f>
         <v>0.54259157105030908</v>
       </c>
+      <c r="Y27" s="45" t="s">
+        <v>1715</v>
+      </c>
+      <c r="Z27" s="31">
+        <f t="shared" ref="Z27:AB27" si="73">Z7/Y7-1</f>
+        <v>1.283844349257111</v>
+      </c>
+      <c r="AA27" s="31">
+        <f t="shared" si="73"/>
+        <v>0.35566940501590616</v>
+      </c>
       <c r="AB27" s="31">
         <f>AB7/AA7-1</f>
         <v>0.48755437773773536</v>
@@ -13239,11 +13624,11 @@
         <v>78</v>
       </c>
       <c r="N28" s="42">
-        <f t="shared" ref="N28:O28" si="44">N7/M7-1</f>
+        <f t="shared" ref="N28:O28" si="74">N7/M7-1</f>
         <v>0.16248573017592149</v>
       </c>
       <c r="O28" s="42">
-        <f t="shared" si="44"/>
+        <f t="shared" si="74"/>
         <v>0.10036762854409043</v>
       </c>
       <c r="P28" s="42">
@@ -13251,15 +13636,15 @@
         <v>3.7070938215102878E-2</v>
       </c>
       <c r="Q28" s="42">
-        <f t="shared" ref="Q28:S28" si="45">Q7/P7-1</f>
+        <f t="shared" ref="Q28:S28" si="75">Q7/P7-1</f>
         <v>0.15782215357458074</v>
       </c>
       <c r="R28" s="42">
-        <f t="shared" si="45"/>
+        <f t="shared" si="75"/>
         <v>6.3647624946400638E-2</v>
       </c>
       <c r="S28" s="42">
-        <f t="shared" si="45"/>
+        <f t="shared" si="75"/>
         <v>7.7769665261658405E-2</v>
       </c>
       <c r="T28" s="42">
@@ -13288,6 +13673,12 @@
       <c r="B31" s="1" t="s">
         <v>1710</v>
       </c>
+      <c r="F31" s="40">
+        <v>64286</v>
+      </c>
+      <c r="J31" s="40">
+        <v>179000</v>
+      </c>
       <c r="M31" s="40">
         <v>208000</v>
       </c>
@@ -13311,6 +13702,14 @@
       </c>
       <c r="T31" s="40">
         <v>275000</v>
+      </c>
+      <c r="Y31" s="40">
+        <f>F31</f>
+        <v>64286</v>
+      </c>
+      <c r="Z31" s="40">
+        <f>J31</f>
+        <v>179000</v>
       </c>
       <c r="AA31" s="40">
         <f>N31</f>
@@ -13325,9 +13724,17 @@
       <c r="B32" s="39" t="s">
         <v>1714</v>
       </c>
+      <c r="J32" s="42">
+        <f t="shared" ref="J32" si="76">J31/F31-1</f>
+        <v>1.7844320691908035</v>
+      </c>
+      <c r="N32" s="42">
+        <f t="shared" ref="N32" si="77">N31/J31-1</f>
+        <v>0.23463687150837997</v>
+      </c>
       <c r="P32" s="41"/>
       <c r="Q32" s="42">
-        <f t="shared" ref="Q32" si="46">Q31/M31-1</f>
+        <f t="shared" ref="Q32" si="78">Q31/M31-1</f>
         <v>0.20192307692307687</v>
       </c>
       <c r="R32" s="42">
@@ -13342,6 +13749,14 @@
         <f>T31/P31-1</f>
         <v>0.14583333333333326</v>
       </c>
+      <c r="Z32" s="42">
+        <f t="shared" ref="Z32:AA32" si="79">Z31/Y31-1</f>
+        <v>1.7844320691908035</v>
+      </c>
+      <c r="AA32" s="42">
+        <f t="shared" si="79"/>
+        <v>0.23463687150837997</v>
+      </c>
       <c r="AB32" s="42">
         <f>AB31/AA31-1</f>
         <v>0.158371040723982</v>
@@ -13352,27 +13767,27 @@
         <v>1713</v>
       </c>
       <c r="N33" s="42">
-        <f t="shared" ref="N33:Q33" si="47">N31/M31-1</f>
+        <f t="shared" ref="N33:Q33" si="80">N31/M31-1</f>
         <v>6.25E-2</v>
       </c>
       <c r="O33" s="42">
-        <f t="shared" si="47"/>
+        <f t="shared" si="80"/>
         <v>6.3348416289592757E-2</v>
       </c>
       <c r="P33" s="42">
-        <f t="shared" si="47"/>
+        <f t="shared" si="80"/>
         <v>2.1276595744680771E-2</v>
       </c>
       <c r="Q33" s="42">
-        <f t="shared" si="47"/>
+        <f t="shared" si="80"/>
         <v>4.1666666666666741E-2</v>
       </c>
       <c r="R33" s="42">
-        <f t="shared" ref="R33:S33" si="48">R31/Q31-1</f>
+        <f t="shared" ref="R33:S33" si="81">R31/Q31-1</f>
         <v>2.4000000000000021E-2</v>
       </c>
       <c r="S33" s="42">
-        <f t="shared" si="48"/>
+        <f t="shared" si="81"/>
         <v>4.6875E-2</v>
       </c>
       <c r="T33" s="42">
@@ -13396,6 +13811,18 @@
       <c r="B34" s="1" t="s">
         <v>1711</v>
       </c>
+      <c r="F34" s="40">
+        <v>1440</v>
+      </c>
+      <c r="G34" s="40"/>
+      <c r="H34" s="40"/>
+      <c r="I34" s="40"/>
+      <c r="J34" s="40">
+        <v>2905</v>
+      </c>
+      <c r="N34" s="40">
+        <v>4629</v>
+      </c>
       <c r="Q34" s="40">
         <v>7381</v>
       </c>
@@ -13409,9 +13836,14 @@
         <v>8510</v>
       </c>
       <c r="V34" s="30"/>
-      <c r="AA34" s="1">
-        <f>N34</f>
-        <v>0</v>
+      <c r="Y34" s="40">
+        <v>1440</v>
+      </c>
+      <c r="Z34" s="40">
+        <v>2905</v>
+      </c>
+      <c r="AA34" s="40">
+        <v>4629</v>
       </c>
       <c r="AB34" s="40">
         <f>R34</f>
@@ -13421,6 +13853,18 @@
     <row r="35" spans="2:28" s="35" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B35" s="39" t="s">
         <v>1712</v>
+      </c>
+      <c r="F35" s="43">
+        <f>F4/F34</f>
+        <v>0.14187638888888887</v>
+      </c>
+      <c r="J35" s="43">
+        <f>J4/J34</f>
+        <v>0.11401858864027538</v>
+      </c>
+      <c r="N35" s="43">
+        <f>N4/N34</f>
+        <v>0.11840354288183194</v>
       </c>
       <c r="P35" s="43"/>
       <c r="Q35" s="43">
@@ -13439,9 +13883,17 @@
         <f>T4/T34</f>
         <v>0.1108524089306698</v>
       </c>
-      <c r="AA35" s="43" t="e">
+      <c r="Y35" s="43">
+        <f t="shared" ref="Y35:Z35" si="82">Y4/Y34</f>
+        <v>0.45143541666666664</v>
+      </c>
+      <c r="Z35" s="43">
+        <f t="shared" si="82"/>
+        <v>0.39052254733218589</v>
+      </c>
+      <c r="AA35" s="43">
         <f>AA4/AA34</f>
-        <v>#DIV/0!</v>
+        <v>0.38059537697126811</v>
       </c>
       <c r="AB35" s="43">
         <f>AB4/AB34</f>
@@ -13457,6 +13909,15 @@
       <c r="B40" s="2" t="s">
         <v>6</v>
       </c>
+      <c r="F40" s="29">
+        <v>487.21499999999997</v>
+      </c>
+      <c r="G40" s="29"/>
+      <c r="H40" s="29"/>
+      <c r="I40" s="29"/>
+      <c r="J40" s="29">
+        <v>253.66</v>
+      </c>
       <c r="N40" s="29">
         <v>933.88499999999999</v>
       </c>
@@ -13471,6 +13932,14 @@
       </c>
       <c r="T40" s="29">
         <v>798.625</v>
+      </c>
+      <c r="Y40" s="29">
+        <f>F40</f>
+        <v>487.21499999999997</v>
+      </c>
+      <c r="Z40" s="29">
+        <f>J40</f>
+        <v>253.66</v>
       </c>
       <c r="AA40" s="29">
         <f>N40</f>
@@ -13485,6 +13954,15 @@
       <c r="B41" s="2" t="s">
         <v>80</v>
       </c>
+      <c r="F41" s="29">
+        <v>261.12799999999999</v>
+      </c>
+      <c r="G41" s="29"/>
+      <c r="H41" s="29"/>
+      <c r="I41" s="29"/>
+      <c r="J41" s="29">
+        <v>1559.0329999999999</v>
+      </c>
       <c r="N41" s="29">
         <v>2105.9059999999999</v>
       </c>
@@ -13500,8 +13978,16 @@
       <c r="T41" s="29">
         <v>3593.6590000000001</v>
       </c>
+      <c r="Y41" s="29">
+        <f t="shared" ref="Y41" si="83">F41</f>
+        <v>261.12799999999999</v>
+      </c>
+      <c r="Z41" s="29">
+        <f t="shared" ref="Z41" si="84">J41</f>
+        <v>1559.0329999999999</v>
+      </c>
       <c r="AA41" s="29">
-        <f t="shared" ref="AA41" si="49">N41</f>
+        <f t="shared" ref="AA41" si="85">N41</f>
         <v>2105.9059999999999</v>
       </c>
       <c r="AB41" s="29">
@@ -13513,6 +13999,15 @@
       <c r="B42" s="1" t="s">
         <v>81</v>
       </c>
+      <c r="F42" s="30">
+        <v>97.712000000000003</v>
+      </c>
+      <c r="G42" s="30"/>
+      <c r="H42" s="30"/>
+      <c r="I42" s="30"/>
+      <c r="J42" s="30">
+        <v>154.06700000000001</v>
+      </c>
       <c r="N42" s="30">
         <v>251.167</v>
       </c>
@@ -13527,6 +14022,14 @@
       </c>
       <c r="T42" s="30">
         <v>471.91500000000002</v>
+      </c>
+      <c r="Y42" s="30">
+        <f>F42</f>
+        <v>97.712000000000003</v>
+      </c>
+      <c r="Z42" s="30">
+        <f>J42</f>
+        <v>154.06700000000001</v>
       </c>
       <c r="AA42" s="30">
         <f>N42</f>
@@ -13541,6 +14044,15 @@
       <c r="B43" s="1" t="s">
         <v>82</v>
       </c>
+      <c r="F43" s="30">
+        <v>26.893000000000001</v>
+      </c>
+      <c r="G43" s="30"/>
+      <c r="H43" s="30"/>
+      <c r="I43" s="30"/>
+      <c r="J43" s="30">
+        <v>54.570999999999998</v>
+      </c>
       <c r="N43" s="30">
         <v>81.376999999999995</v>
       </c>
@@ -13556,12 +14068,20 @@
       <c r="T43" s="30">
         <v>240.19200000000001</v>
       </c>
+      <c r="Y43" s="30">
+        <f t="shared" ref="Y43" si="86">F43</f>
+        <v>26.893000000000001</v>
+      </c>
+      <c r="Z43" s="30">
+        <f t="shared" ref="Z43" si="87">J43</f>
+        <v>54.570999999999998</v>
+      </c>
       <c r="AA43" s="30">
-        <f t="shared" ref="AA43" si="50">N43</f>
+        <f t="shared" ref="AA43" si="88">N43</f>
         <v>81.376999999999995</v>
       </c>
       <c r="AB43" s="30">
-        <f t="shared" ref="AB43" si="51">R43</f>
+        <f t="shared" ref="AB43" si="89">R43</f>
         <v>186.131</v>
       </c>
     </row>
@@ -13569,6 +14089,17 @@
       <c r="B44" s="1" t="s">
         <v>83</v>
       </c>
+      <c r="F44" s="30">
+        <f>SUM(F40:F43)</f>
+        <v>872.94799999999998</v>
+      </c>
+      <c r="G44" s="30"/>
+      <c r="H44" s="30"/>
+      <c r="I44" s="30"/>
+      <c r="J44" s="30">
+        <f>SUM(J40:J43)</f>
+        <v>2021.3309999999999</v>
+      </c>
       <c r="N44" s="30">
         <f>SUM(N40:N43)</f>
         <v>3372.335</v>
@@ -13589,12 +14120,20 @@
         <f>SUM(T40:T43)</f>
         <v>5104.3909999999996</v>
       </c>
+      <c r="Y44" s="30">
+        <f t="shared" ref="Y44:AB44" si="90">SUM(Y40:Y43)</f>
+        <v>872.94799999999998</v>
+      </c>
+      <c r="Z44" s="30">
+        <f t="shared" si="90"/>
+        <v>2021.3309999999999</v>
+      </c>
       <c r="AA44" s="30">
-        <f t="shared" ref="AA44:AB44" si="52">SUM(AA40:AA43)</f>
+        <f t="shared" si="90"/>
         <v>3372.335</v>
       </c>
       <c r="AB44" s="30">
-        <f t="shared" si="52"/>
+        <f t="shared" si="90"/>
         <v>5932.2280000000001</v>
       </c>
     </row>
@@ -13602,6 +14141,15 @@
       <c r="B45" s="1" t="s">
         <v>84</v>
       </c>
+      <c r="F45" s="30">
+        <v>63.533999999999999</v>
+      </c>
+      <c r="G45" s="30"/>
+      <c r="H45" s="30"/>
+      <c r="I45" s="30"/>
+      <c r="J45" s="30">
+        <v>141.256</v>
+      </c>
       <c r="N45" s="30">
         <v>183.239</v>
       </c>
@@ -13617,12 +14165,20 @@
       <c r="T45" s="30">
         <v>264.767</v>
       </c>
+      <c r="Y45" s="30">
+        <f t="shared" ref="Y45:Y49" si="91">F45</f>
+        <v>63.533999999999999</v>
+      </c>
+      <c r="Z45" s="30">
+        <f>J45</f>
+        <v>141.256</v>
+      </c>
       <c r="AA45" s="30">
-        <f t="shared" ref="AA45:AA49" si="53">N45</f>
+        <f t="shared" ref="AA45:AA49" si="92">N45</f>
         <v>183.239</v>
       </c>
       <c r="AB45" s="30">
-        <f t="shared" ref="AB45:AB49" si="54">R45</f>
+        <f t="shared" ref="AB45:AB49" si="93">R45</f>
         <v>255.316</v>
       </c>
     </row>
@@ -13630,6 +14186,15 @@
       <c r="B46" s="1" t="s">
         <v>85</v>
       </c>
+      <c r="F46" s="30">
+        <v>0</v>
+      </c>
+      <c r="G46" s="30"/>
+      <c r="H46" s="30"/>
+      <c r="I46" s="30"/>
+      <c r="J46" s="30">
+        <v>156.74100000000001</v>
+      </c>
       <c r="N46" s="30">
         <v>258.61</v>
       </c>
@@ -13645,12 +14210,20 @@
       <c r="T46" s="30">
         <v>213.464</v>
       </c>
+      <c r="Y46" s="30">
+        <f t="shared" si="91"/>
+        <v>0</v>
+      </c>
+      <c r="Z46" s="30">
+        <f>J45</f>
+        <v>141.256</v>
+      </c>
       <c r="AA46" s="30">
-        <f t="shared" si="53"/>
+        <f t="shared" si="92"/>
         <v>258.61</v>
       </c>
       <c r="AB46" s="30">
-        <f t="shared" si="54"/>
+        <f t="shared" si="93"/>
         <v>234.584</v>
       </c>
     </row>
@@ -13658,6 +14231,15 @@
       <c r="B47" s="1" t="s">
         <v>86</v>
       </c>
+      <c r="F47" s="30">
+        <v>18.119</v>
+      </c>
+      <c r="G47" s="30"/>
+      <c r="H47" s="30"/>
+      <c r="I47" s="30"/>
+      <c r="J47" s="30">
+        <v>7.4999999999999997E-2</v>
+      </c>
       <c r="N47" s="30">
         <v>0</v>
       </c>
@@ -13673,12 +14255,20 @@
       <c r="T47" s="30">
         <v>750</v>
       </c>
+      <c r="Y47" s="30">
+        <f t="shared" si="91"/>
+        <v>18.119</v>
+      </c>
+      <c r="Z47" s="30">
+        <f>J47</f>
+        <v>7.4999999999999997E-2</v>
+      </c>
       <c r="AA47" s="30">
-        <f t="shared" si="53"/>
+        <f t="shared" si="92"/>
         <v>0</v>
       </c>
       <c r="AB47" s="30">
-        <f t="shared" si="54"/>
+        <f t="shared" si="93"/>
         <v>0</v>
       </c>
     </row>
@@ -13686,6 +14276,17 @@
       <c r="B48" s="1" t="s">
         <v>87</v>
       </c>
+      <c r="F48" s="30">
+        <f>27.558+38.165</f>
+        <v>65.722999999999999</v>
+      </c>
+      <c r="G48" s="30"/>
+      <c r="H48" s="30"/>
+      <c r="I48" s="30"/>
+      <c r="J48" s="30">
+        <f>480.849+2296.784</f>
+        <v>2777.6330000000003</v>
+      </c>
       <c r="N48" s="30">
         <f>966.573+4595.394</f>
         <v>5561.9670000000006</v>
@@ -13706,12 +14307,20 @@
         <f>953.522+5285.563</f>
         <v>6239.085</v>
       </c>
+      <c r="Y48" s="30">
+        <f t="shared" si="91"/>
+        <v>65.722999999999999</v>
+      </c>
+      <c r="Z48" s="30">
+        <f t="shared" ref="Z45:Z49" si="94">J48</f>
+        <v>2777.6330000000003</v>
+      </c>
       <c r="AA48" s="30">
-        <f t="shared" si="53"/>
+        <f t="shared" si="92"/>
         <v>5561.9670000000006</v>
       </c>
       <c r="AB48" s="30">
-        <f t="shared" si="54"/>
+        <f t="shared" si="93"/>
         <v>6313.1779999999999</v>
       </c>
     </row>
@@ -13719,6 +14328,15 @@
       <c r="B49" s="1" t="s">
         <v>88</v>
       </c>
+      <c r="F49" s="30">
+        <v>8.3859999999999992</v>
+      </c>
+      <c r="G49" s="30"/>
+      <c r="H49" s="30"/>
+      <c r="I49" s="30"/>
+      <c r="J49" s="30">
+        <v>33.479999999999997</v>
+      </c>
       <c r="N49" s="30">
         <v>111.282</v>
       </c>
@@ -13734,12 +14352,20 @@
       <c r="T49" s="30">
         <v>297.52199999999999</v>
       </c>
+      <c r="Y49" s="30">
+        <f t="shared" si="91"/>
+        <v>8.3859999999999992</v>
+      </c>
+      <c r="Z49" s="30">
+        <f t="shared" si="94"/>
+        <v>33.479999999999997</v>
+      </c>
       <c r="AA49" s="30">
-        <f t="shared" si="53"/>
+        <f t="shared" si="92"/>
         <v>111.282</v>
       </c>
       <c r="AB49" s="30">
-        <f t="shared" si="54"/>
+        <f t="shared" si="93"/>
         <v>263.29199999999997</v>
       </c>
     </row>
@@ -13747,6 +14373,17 @@
       <c r="B50" s="1" t="s">
         <v>89</v>
       </c>
+      <c r="F50" s="30">
+        <f>F44+SUM(F45:F49)</f>
+        <v>1028.71</v>
+      </c>
+      <c r="G50" s="30"/>
+      <c r="H50" s="30"/>
+      <c r="I50" s="30"/>
+      <c r="J50" s="30">
+        <f>J44+SUM(J45:J49)</f>
+        <v>5130.5160000000005</v>
+      </c>
       <c r="N50" s="30">
         <f>N44+SUM(N45:N49)</f>
         <v>9487.4330000000009</v>
@@ -13767,12 +14404,20 @@
         <f>T44+SUM(T45:T49)</f>
         <v>12869.228999999999</v>
       </c>
+      <c r="Y50" s="30">
+        <f t="shared" ref="Y50:AB50" si="95">Y44+SUM(Y45:Y49)</f>
+        <v>1028.71</v>
+      </c>
+      <c r="Z50" s="30">
+        <f t="shared" si="95"/>
+        <v>5115.0309999999999</v>
+      </c>
       <c r="AA50" s="30">
-        <f t="shared" ref="AA50:AB50" si="55">AA44+SUM(AA45:AA49)</f>
+        <f t="shared" si="95"/>
         <v>9487.4330000000009</v>
       </c>
       <c r="AB50" s="30">
-        <f t="shared" si="55"/>
+        <f t="shared" si="95"/>
         <v>12998.598</v>
       </c>
     </row>
@@ -13781,11 +14426,19 @@
       <c r="Q51" s="30"/>
       <c r="S51" s="30"/>
       <c r="T51" s="30"/>
+      <c r="Y51" s="30"/>
+      <c r="Z51" s="30"/>
     </row>
     <row r="52" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B52" s="1" t="s">
         <v>90</v>
       </c>
+      <c r="F52" s="30">
+        <v>18.495000000000001</v>
+      </c>
+      <c r="J52" s="30">
+        <v>39.098999999999997</v>
+      </c>
       <c r="N52" s="30">
         <v>60.042000000000002</v>
       </c>
@@ -13801,12 +14454,20 @@
       <c r="T52" s="30">
         <v>102.039</v>
       </c>
+      <c r="Y52" s="30">
+        <f t="shared" ref="Y52:Y55" si="96">F52</f>
+        <v>18.495000000000001</v>
+      </c>
+      <c r="Z52" s="30">
+        <f t="shared" ref="Z52:Z55" si="97">J52</f>
+        <v>39.098999999999997</v>
+      </c>
       <c r="AA52" s="30">
-        <f t="shared" ref="AA52:AA57" si="56">N52</f>
+        <f t="shared" ref="Y52:AB58" si="98">N52</f>
         <v>60.042000000000002</v>
       </c>
       <c r="AB52" s="30">
-        <f t="shared" ref="AB52:AB55" si="57">R52</f>
+        <f t="shared" ref="AB52:AB55" si="99">R52</f>
         <v>93.332999999999998</v>
       </c>
     </row>
@@ -13814,6 +14475,12 @@
       <c r="B53" s="1" t="s">
         <v>91</v>
       </c>
+      <c r="F53" s="30">
+        <v>96.343000000000004</v>
+      </c>
+      <c r="J53" s="30">
+        <v>147.68100000000001</v>
+      </c>
       <c r="N53" s="30">
         <v>252.89500000000001</v>
       </c>
@@ -13829,12 +14496,20 @@
       <c r="T53" s="30">
         <v>504.81</v>
       </c>
+      <c r="Y53" s="30">
+        <f t="shared" si="96"/>
+        <v>96.343000000000004</v>
+      </c>
+      <c r="Z53" s="30">
+        <f t="shared" si="97"/>
+        <v>147.68100000000001</v>
+      </c>
       <c r="AA53" s="30">
-        <f t="shared" si="56"/>
+        <f t="shared" si="98"/>
         <v>252.89500000000001</v>
       </c>
       <c r="AB53" s="30">
-        <f t="shared" si="57"/>
+        <f t="shared" si="99"/>
         <v>417.50299999999999</v>
       </c>
     </row>
@@ -13842,6 +14517,12 @@
       <c r="B54" s="1" t="s">
         <v>92</v>
       </c>
+      <c r="F54" s="30">
+        <v>22.972000000000001</v>
+      </c>
+      <c r="J54" s="30">
+        <v>26.361999999999998</v>
+      </c>
       <c r="N54" s="30">
         <v>87.031000000000006</v>
       </c>
@@ -13857,12 +14538,20 @@
       <c r="T54" s="30">
         <v>137.72800000000001</v>
       </c>
+      <c r="Y54" s="30">
+        <f t="shared" si="96"/>
+        <v>22.972000000000001</v>
+      </c>
+      <c r="Z54" s="30">
+        <f t="shared" si="97"/>
+        <v>26.361999999999998</v>
+      </c>
       <c r="AA54" s="30">
-        <f t="shared" si="56"/>
+        <f t="shared" si="98"/>
         <v>87.031000000000006</v>
       </c>
       <c r="AB54" s="30">
-        <f t="shared" si="57"/>
+        <f t="shared" si="99"/>
         <v>140.38900000000001</v>
       </c>
     </row>
@@ -13870,6 +14559,12 @@
       <c r="B55" s="1" t="s">
         <v>93</v>
       </c>
+      <c r="F55" s="30">
+        <v>0</v>
+      </c>
+      <c r="J55" s="30">
+        <v>27.155999999999999</v>
+      </c>
       <c r="N55" s="30">
         <v>48.338000000000001</v>
       </c>
@@ -13885,630 +14580,968 @@
       <c r="T55" s="30">
         <v>50.743000000000002</v>
       </c>
+      <c r="Y55" s="30">
+        <f t="shared" si="96"/>
+        <v>0</v>
+      </c>
+      <c r="Z55" s="30">
+        <f t="shared" si="97"/>
+        <v>27.155999999999999</v>
+      </c>
       <c r="AA55" s="30">
-        <f t="shared" si="56"/>
+        <f t="shared" si="98"/>
         <v>48.338000000000001</v>
       </c>
       <c r="AB55" s="30">
-        <f t="shared" si="57"/>
+        <f t="shared" si="99"/>
         <v>52.325000000000003</v>
       </c>
     </row>
     <row r="56" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B56" s="1" t="s">
-        <v>94</v>
+        <v>95</v>
+      </c>
+      <c r="F56" s="30">
+        <v>0</v>
+      </c>
+      <c r="J56" s="30">
+        <v>6.9240000000000004</v>
       </c>
       <c r="N56" s="30">
-        <f>SUM(N52:N55)</f>
-        <v>448.30600000000004</v>
+        <v>0</v>
       </c>
       <c r="Q56" s="30">
-        <v>617.07299999999998</v>
+        <v>0</v>
       </c>
       <c r="R56" s="30">
-        <f>SUM(R52:R55)</f>
-        <v>703.55000000000007</v>
+        <v>0</v>
       </c>
       <c r="S56" s="30">
-        <f>SUM(S52:S55)</f>
-        <v>719.82200000000012</v>
+        <v>0</v>
       </c>
       <c r="T56" s="30">
-        <f>SUM(T52:T55)</f>
-        <v>795.32</v>
+        <v>0</v>
+      </c>
+      <c r="Y56" s="30">
+        <f>F56</f>
+        <v>0</v>
+      </c>
+      <c r="Z56" s="30">
+        <f>J56</f>
+        <v>6.9240000000000004</v>
       </c>
       <c r="AA56" s="30">
-        <f t="shared" ref="AA56:AB56" si="58">SUM(AA52:AA55)</f>
-        <v>448.30600000000004</v>
+        <f t="shared" si="98"/>
+        <v>0</v>
       </c>
       <c r="AB56" s="30">
-        <f t="shared" si="58"/>
-        <v>703.55000000000007</v>
+        <f>R56</f>
+        <v>0</v>
       </c>
     </row>
     <row r="57" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B57" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="F57" s="30">
+        <f>SUM(F52:F56)</f>
+        <v>137.81</v>
+      </c>
+      <c r="J57" s="30">
+        <f>SUM(J52:J56)</f>
+        <v>247.22200000000001</v>
+      </c>
+      <c r="N57" s="30">
+        <f>SUM(N52:N56)</f>
+        <v>448.30600000000004</v>
+      </c>
+      <c r="Q57" s="30">
+        <f t="shared" ref="Q57:S57" si="100">SUM(Q52:Q56)</f>
+        <v>617.25300000000004</v>
+      </c>
+      <c r="R57" s="30">
+        <f t="shared" si="100"/>
+        <v>703.55000000000007</v>
+      </c>
+      <c r="S57" s="30">
+        <f t="shared" si="100"/>
+        <v>719.82200000000012</v>
+      </c>
+      <c r="T57" s="30">
+        <f>SUM(T52:T56)</f>
+        <v>795.32</v>
+      </c>
+      <c r="Y57" s="30">
+        <f>SUM(Y52:Y56)</f>
+        <v>137.81</v>
+      </c>
+      <c r="Z57" s="30">
+        <f>SUM(Z52:Z56)</f>
+        <v>247.22200000000001</v>
+      </c>
+      <c r="AA57" s="30">
+        <f>SUM(AA52:AA56)</f>
+        <v>448.30600000000004</v>
+      </c>
+      <c r="AB57" s="30">
+        <f>SUM(AB52:AB56)</f>
+        <v>703.55000000000007</v>
+      </c>
+    </row>
+    <row r="58" spans="2:28" x14ac:dyDescent="0.2">
+      <c r="B58" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="N57" s="30">
+      <c r="F58" s="30">
+        <v>0</v>
+      </c>
+      <c r="J58" s="30">
+        <v>139.19999999999999</v>
+      </c>
+      <c r="N58" s="30">
         <v>229.905</v>
       </c>
-      <c r="Q57" s="30">
+      <c r="Q58" s="30">
         <v>223.03299999999999</v>
       </c>
-      <c r="R57" s="30">
+      <c r="R58" s="30">
         <v>211.25299999999999</v>
       </c>
-      <c r="S57" s="30">
+      <c r="S58" s="30">
         <v>201.35400000000001</v>
       </c>
-      <c r="T57" s="30">
+      <c r="T58" s="30">
         <v>189.06800000000001</v>
       </c>
-      <c r="AA57" s="30">
-        <f t="shared" si="56"/>
+      <c r="Y58" s="30">
+        <f t="shared" ref="Y58:Y61" si="101">F58</f>
+        <v>0</v>
+      </c>
+      <c r="Z58" s="30">
+        <f t="shared" ref="Z58:Z61" si="102">J58</f>
+        <v>139.19999999999999</v>
+      </c>
+      <c r="AA58" s="30">
+        <f t="shared" si="98"/>
         <v>229.905</v>
       </c>
-      <c r="AB57" s="30">
-        <f t="shared" ref="AB57" si="59">R57</f>
+      <c r="AB58" s="30">
+        <f t="shared" ref="AB58" si="103">R58</f>
         <v>211.25299999999999</v>
-      </c>
-    </row>
-    <row r="58" spans="2:28" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B58" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="N58" s="29">
-        <v>17.856000000000002</v>
-      </c>
-      <c r="Q58" s="29">
-        <v>20.254000000000001</v>
-      </c>
-      <c r="R58" s="29">
-        <v>25.132000000000001</v>
-      </c>
-      <c r="S58" s="29">
-        <v>22.053000000000001</v>
-      </c>
-      <c r="T58" s="29">
-        <v>18.934999999999999</v>
-      </c>
-      <c r="AA58" s="29">
-        <f t="shared" ref="AA58" si="60">N58</f>
-        <v>17.856000000000002</v>
-      </c>
-      <c r="AB58" s="29">
-        <f>R58</f>
-        <v>25.132000000000001</v>
       </c>
     </row>
     <row r="59" spans="2:28" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B59" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="F59" s="29">
+        <v>0</v>
+      </c>
+      <c r="J59" s="29">
+        <v>8.7460000000000004</v>
+      </c>
+      <c r="N59" s="29">
+        <v>17.856000000000002</v>
+      </c>
+      <c r="Q59" s="29">
+        <v>20.254000000000001</v>
+      </c>
+      <c r="R59" s="29">
+        <v>25.132000000000001</v>
+      </c>
+      <c r="S59" s="29">
+        <v>22.053000000000001</v>
+      </c>
+      <c r="T59" s="29">
+        <v>18.934999999999999</v>
+      </c>
+      <c r="Y59" s="29">
+        <f t="shared" si="101"/>
+        <v>0</v>
+      </c>
+      <c r="Z59" s="29">
+        <f t="shared" si="102"/>
+        <v>8.7460000000000004</v>
+      </c>
+      <c r="AA59" s="29">
+        <f t="shared" ref="AA59" si="104">N59</f>
+        <v>17.856000000000002</v>
+      </c>
+      <c r="AB59" s="29">
+        <f>R59</f>
+        <v>25.132000000000001</v>
+      </c>
+    </row>
+    <row r="60" spans="2:28" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B60" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="N59" s="29">
+      <c r="F60" s="29">
+        <v>434.49599999999998</v>
+      </c>
+      <c r="J60" s="29">
+        <v>458.19</v>
+      </c>
+      <c r="N60" s="29">
         <v>302.06799999999998</v>
       </c>
-      <c r="Q59" s="29">
+      <c r="Q60" s="29">
         <v>985.54700000000003</v>
       </c>
-      <c r="R59" s="29">
+      <c r="R60" s="29">
         <v>985.90700000000004</v>
       </c>
-      <c r="S59" s="29">
+      <c r="S60" s="29">
         <v>986.24300000000005</v>
       </c>
-      <c r="T59" s="29">
+      <c r="T60" s="29">
         <v>986.61900000000003</v>
       </c>
-      <c r="AA59" s="29">
-        <f t="shared" ref="AA59:AA60" si="61">N59</f>
+      <c r="Y60" s="29">
+        <f t="shared" si="101"/>
+        <v>434.49599999999998</v>
+      </c>
+      <c r="Z60" s="29">
+        <f t="shared" si="102"/>
+        <v>458.19</v>
+      </c>
+      <c r="AA60" s="29">
+        <f t="shared" ref="AA60:AA61" si="105">N60</f>
         <v>302.06799999999998</v>
       </c>
-      <c r="AB59" s="29">
-        <f t="shared" ref="AB59:AB60" si="62">R59</f>
+      <c r="AB60" s="29">
+        <f t="shared" ref="AB60:AB61" si="106">R60</f>
         <v>985.90700000000004</v>
-      </c>
-    </row>
-    <row r="60" spans="2:28" x14ac:dyDescent="0.2">
-      <c r="B60" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="N60" s="30">
-        <v>36.633000000000003</v>
-      </c>
-      <c r="Q60" s="30">
-        <v>49.191000000000003</v>
-      </c>
-      <c r="R60" s="30">
-        <v>41.29</v>
-      </c>
-      <c r="S60" s="30">
-        <v>43.896999999999998</v>
-      </c>
-      <c r="T60" s="30">
-        <v>37.292000000000002</v>
-      </c>
-      <c r="AA60" s="30">
-        <f t="shared" si="61"/>
-        <v>36.633000000000003</v>
-      </c>
-      <c r="AB60" s="30">
-        <f t="shared" si="62"/>
-        <v>41.29</v>
       </c>
     </row>
     <row r="61" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B61" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="F61" s="30">
+        <v>18.169</v>
+      </c>
+      <c r="J61" s="30">
+        <v>17.747</v>
+      </c>
+      <c r="N61" s="30">
+        <v>36.633000000000003</v>
+      </c>
+      <c r="Q61" s="30">
+        <v>49.191000000000003</v>
+      </c>
+      <c r="R61" s="30">
+        <v>41.29</v>
+      </c>
+      <c r="S61" s="30">
+        <v>43.896999999999998</v>
+      </c>
+      <c r="T61" s="30">
+        <v>37.292000000000002</v>
+      </c>
+      <c r="Y61" s="30">
+        <f t="shared" si="101"/>
+        <v>18.169</v>
+      </c>
+      <c r="Z61" s="30">
+        <f t="shared" si="102"/>
+        <v>17.747</v>
+      </c>
+      <c r="AA61" s="30">
+        <f t="shared" si="105"/>
+        <v>36.633000000000003</v>
+      </c>
+      <c r="AB61" s="30">
+        <f t="shared" si="106"/>
+        <v>41.29</v>
+      </c>
+    </row>
+    <row r="62" spans="2:28" x14ac:dyDescent="0.2">
+      <c r="B62" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="N61" s="30">
-        <f>SUM(N57:N60)+N56</f>
+      <c r="F62" s="30">
+        <f>SUM(F58:F61)+F57</f>
+        <v>590.47499999999991</v>
+      </c>
+      <c r="J62" s="30">
+        <f>SUM(J58:J61)+J57</f>
+        <v>871.1049999999999</v>
+      </c>
+      <c r="N62" s="30">
+        <f>SUM(N58:N61)+N57</f>
         <v>1034.768</v>
       </c>
-      <c r="Q61" s="30">
-        <f>SUM(Q57:Q60)+Q56</f>
-        <v>1895.098</v>
-      </c>
-      <c r="R61" s="30">
-        <f>SUM(R57:R60)+R56</f>
+      <c r="Q62" s="30">
+        <f>SUM(Q58:Q61)+Q57</f>
+        <v>1895.2780000000002</v>
+      </c>
+      <c r="R62" s="30">
+        <f>SUM(R58:R61)+R57</f>
         <v>1967.1320000000001</v>
       </c>
-      <c r="S61" s="30">
-        <f>SUM(S57:S60)+S56</f>
+      <c r="S62" s="30">
+        <f>SUM(S58:S61)+S57</f>
         <v>1973.3690000000001</v>
       </c>
-      <c r="T61" s="30">
-        <f>SUM(T57:T60)+T56</f>
+      <c r="T62" s="30">
+        <f>SUM(T58:T61)+T57</f>
         <v>2027.2339999999999</v>
       </c>
-      <c r="AA61" s="30">
-        <f>SUM(AA57:AA60)+AA56</f>
+      <c r="Y62" s="30">
+        <f t="shared" ref="Y62:Z62" si="107">SUM(Y58:Y61)+Y57</f>
+        <v>590.47499999999991</v>
+      </c>
+      <c r="Z62" s="30">
+        <f t="shared" si="107"/>
+        <v>871.1049999999999</v>
+      </c>
+      <c r="AA62" s="30">
+        <f>SUM(AA58:AA61)+AA57</f>
         <v>1034.768</v>
       </c>
-      <c r="AB61" s="30">
-        <f>SUM(AB57:AB60)+AB56</f>
+      <c r="AB62" s="30">
+        <f>SUM(AB58:AB61)+AB57</f>
         <v>1967.1320000000001</v>
       </c>
     </row>
-    <row r="62" spans="2:28" x14ac:dyDescent="0.2">
-      <c r="T62" s="30"/>
-    </row>
     <row r="63" spans="2:28" x14ac:dyDescent="0.2">
-      <c r="B63" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="N63" s="30">
-        <v>8452.6650000000009</v>
-      </c>
-      <c r="Q63" s="30">
-        <v>11081.749</v>
-      </c>
-      <c r="R63" s="30">
-        <v>11031.466</v>
-      </c>
-      <c r="S63" s="30">
-        <v>10917.433000000001</v>
-      </c>
-      <c r="T63" s="30">
-        <v>10841.995000000001</v>
-      </c>
-      <c r="AA63" s="30">
-        <f>N63</f>
-        <v>8452.6650000000009</v>
-      </c>
-      <c r="AB63" s="30">
-        <f>R63</f>
-        <v>11031.466</v>
-      </c>
+      <c r="T63" s="30"/>
+      <c r="Y63" s="30"/>
+      <c r="Z63" s="30"/>
     </row>
     <row r="64" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B64" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="F64" s="30">
+        <v>438.23500000000001</v>
+      </c>
+      <c r="J64" s="30">
+        <v>4279.4110000000001</v>
+      </c>
+      <c r="N64" s="30">
+        <v>8452.6650000000009</v>
+      </c>
+      <c r="Q64" s="30">
+        <v>11081.749</v>
+      </c>
+      <c r="R64" s="30">
+        <v>11031.466</v>
+      </c>
+      <c r="S64" s="30">
+        <v>10917.433000000001</v>
+      </c>
+      <c r="T64" s="30">
+        <v>10841.995000000001</v>
+      </c>
+      <c r="Y64" s="30">
+        <f>F64</f>
+        <v>438.23500000000001</v>
+      </c>
+      <c r="Z64" s="30">
+        <f>J64</f>
+        <v>4279.4110000000001</v>
+      </c>
+      <c r="AA64" s="30">
+        <f>N64</f>
+        <v>8452.6650000000009</v>
+      </c>
+      <c r="AB64" s="30">
+        <f>R64</f>
+        <v>11031.466</v>
+      </c>
+    </row>
+    <row r="65" spans="2:28" x14ac:dyDescent="0.2">
+      <c r="B65" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="N64" s="30">
-        <f>N63+N61</f>
+      <c r="F65" s="30">
+        <f>F64+F62</f>
+        <v>1028.71</v>
+      </c>
+      <c r="J65" s="30">
+        <f>J64+J62</f>
+        <v>5150.5159999999996</v>
+      </c>
+      <c r="N65" s="30">
+        <f>N64+N62</f>
         <v>9487.4330000000009</v>
       </c>
-      <c r="Q64" s="30">
-        <f>Q63+Q61</f>
-        <v>12976.847</v>
-      </c>
-      <c r="R64" s="30">
-        <f>R63+R61</f>
+      <c r="Q65" s="30">
+        <f>Q64+Q62</f>
+        <v>12977.027</v>
+      </c>
+      <c r="R65" s="30">
+        <f>R64+R62</f>
         <v>12998.598</v>
       </c>
-      <c r="S64" s="30">
-        <f>S63+S61</f>
+      <c r="S65" s="30">
+        <f>S64+S62</f>
         <v>12890.802000000001</v>
       </c>
-      <c r="T64" s="30">
-        <f>T63+T61</f>
+      <c r="T65" s="30">
+        <f>T64+T62</f>
         <v>12869.229000000001</v>
       </c>
-      <c r="AA64" s="30">
-        <f>AA63+AA61</f>
+      <c r="Y65" s="30">
+        <f>Y64+Y62</f>
+        <v>1028.71</v>
+      </c>
+      <c r="Z65" s="30">
+        <f>Z64+Z62</f>
+        <v>5150.5159999999996</v>
+      </c>
+      <c r="AA65" s="30">
+        <f>AA64+AA62</f>
         <v>9487.4330000000009</v>
       </c>
-      <c r="AB64" s="30">
-        <f>AB63+AB61</f>
+      <c r="AB65" s="30">
+        <f>AB64+AB62</f>
         <v>12998.598</v>
       </c>
     </row>
     <row r="66" spans="2:28" x14ac:dyDescent="0.2">
-      <c r="B66" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="N66" s="30">
-        <f t="shared" ref="N66" si="63">N50-N61</f>
-        <v>8452.6650000000009</v>
-      </c>
-      <c r="Q66" s="30">
-        <f t="shared" ref="Q66:R66" si="64">Q50-Q61</f>
-        <v>11081.749000000002</v>
-      </c>
-      <c r="R66" s="30">
-        <f t="shared" si="64"/>
-        <v>11031.466</v>
-      </c>
-      <c r="S66" s="30">
-        <f t="shared" ref="S66" si="65">S50-S61</f>
-        <v>10917.432999999999</v>
-      </c>
-      <c r="T66" s="30">
-        <f>T50-T61</f>
-        <v>10841.994999999999</v>
-      </c>
-      <c r="AA66" s="30">
-        <f>AA50-AA61</f>
-        <v>8452.6650000000009</v>
-      </c>
-      <c r="AB66" s="30">
-        <f>AB50-AB61</f>
-        <v>11031.466</v>
-      </c>
+      <c r="Y66" s="30"/>
+      <c r="Z66" s="30"/>
     </row>
     <row r="67" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B67" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="F67" s="30">
+        <f t="shared" ref="F67" si="108">F50-F62</f>
+        <v>438.23500000000013</v>
+      </c>
+      <c r="J67" s="30">
+        <f t="shared" ref="J67" si="109">J50-J62</f>
+        <v>4259.411000000001</v>
+      </c>
+      <c r="N67" s="30">
+        <f t="shared" ref="N67" si="110">N50-N62</f>
+        <v>8452.6650000000009</v>
+      </c>
+      <c r="Q67" s="30">
+        <f t="shared" ref="Q67:R67" si="111">Q50-Q62</f>
+        <v>11081.569000000001</v>
+      </c>
+      <c r="R67" s="30">
+        <f t="shared" si="111"/>
+        <v>11031.466</v>
+      </c>
+      <c r="S67" s="30">
+        <f t="shared" ref="S67" si="112">S50-S62</f>
+        <v>10917.432999999999</v>
+      </c>
+      <c r="T67" s="30">
+        <f>T50-T62</f>
+        <v>10841.994999999999</v>
+      </c>
+      <c r="Y67" s="30">
+        <f>Y50-Y62</f>
+        <v>438.23500000000013</v>
+      </c>
+      <c r="Z67" s="30">
+        <f>Z50-Z62</f>
+        <v>4243.9260000000004</v>
+      </c>
+      <c r="AA67" s="30">
+        <f>AA50-AA62</f>
+        <v>8452.6650000000009</v>
+      </c>
+      <c r="AB67" s="30">
+        <f>AB50-AB62</f>
+        <v>11031.466</v>
+      </c>
+    </row>
+    <row r="68" spans="2:28" x14ac:dyDescent="0.2">
+      <c r="B68" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="N67" s="1">
-        <f t="shared" ref="N67" si="66">N66/N17</f>
+      <c r="F68" s="1">
+        <f t="shared" ref="F68" si="113">F67/F17</f>
+        <v>4.4080086658029467</v>
+      </c>
+      <c r="J68" s="1">
+        <f t="shared" ref="J68" si="114">J67/J17</f>
+        <v>30.926123407736053</v>
+      </c>
+      <c r="N68" s="1">
+        <f t="shared" ref="N68" si="115">N67/N17</f>
         <v>53.368623979541908</v>
       </c>
-      <c r="Q67" s="1">
-        <f t="shared" ref="Q67" si="67">Q66/Q17</f>
-        <v>62.527047637215972</v>
-      </c>
-      <c r="R67" s="1">
-        <f t="shared" ref="R67" si="68">R66/R17</f>
+      <c r="Q68" s="1">
+        <f t="shared" ref="Q68" si="116">Q67/Q17</f>
+        <v>62.526032015171587</v>
+      </c>
+      <c r="R68" s="1">
+        <f t="shared" ref="R68" si="117">R67/R17</f>
         <v>61.650794916840383</v>
       </c>
-      <c r="S67" s="1">
-        <f t="shared" ref="S67" si="69">S66/S17</f>
+      <c r="S68" s="1">
+        <f t="shared" ref="S68" si="118">S67/S17</f>
         <v>60.351081657501894</v>
       </c>
-      <c r="T67" s="1">
-        <f>T66/T17</f>
+      <c r="T68" s="1">
+        <f>T67/T17</f>
         <v>59.457757070299436</v>
       </c>
-      <c r="AA67" s="1">
-        <f>AA66/AA17</f>
+      <c r="Y68" s="1">
+        <f>Y67/Y17</f>
+        <v>4.511824055303669</v>
+      </c>
+      <c r="Z68" s="1">
+        <f>Z67/Z17</f>
+        <v>32.624743427364088</v>
+      </c>
+      <c r="AA68" s="1">
+        <f>AA67/AA17</f>
         <v>57.615309329074869</v>
       </c>
-      <c r="AB67" s="1">
-        <f>AB66/AB17</f>
+      <c r="AB68" s="1">
+        <f>AB67/AB17</f>
         <v>63.333543173168131</v>
       </c>
     </row>
-    <row r="69" spans="2:28" s="35" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B69" s="35" t="s">
+    <row r="69" spans="2:28" x14ac:dyDescent="0.2">
+      <c r="Y69" s="30"/>
+      <c r="Z69" s="30"/>
+    </row>
+    <row r="70" spans="2:28" s="35" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B70" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="N69" s="36">
+      <c r="F70" s="36">
+        <f>F40+F41</f>
+        <v>748.34299999999996</v>
+      </c>
+      <c r="J70" s="36">
+        <f>J40+J41</f>
+        <v>1812.693</v>
+      </c>
+      <c r="N70" s="36">
         <f>N40+N41</f>
         <v>3039.7910000000002</v>
       </c>
-      <c r="Q69" s="36">
-        <f t="shared" ref="Q69" si="70">Q40+Q41</f>
+      <c r="Q70" s="36">
+        <f t="shared" ref="Q70" si="119">Q40+Q41</f>
         <v>5394.2520000000004</v>
       </c>
-      <c r="R69" s="36">
+      <c r="R70" s="36">
         <f>R40+R41</f>
         <v>5357.8819999999996</v>
       </c>
-      <c r="S69" s="36">
+      <c r="S70" s="36">
         <f>S40+S41</f>
         <v>5223.3119999999999</v>
       </c>
-      <c r="T69" s="36">
+      <c r="T70" s="36">
         <f>T40+T41</f>
         <v>4392.2839999999997</v>
       </c>
-      <c r="AA69" s="36">
-        <f>N69</f>
-        <v>3039.7910000000002</v>
-      </c>
-      <c r="AB69" s="36">
-        <f>R69</f>
-        <v>5357.8819999999996</v>
-      </c>
-    </row>
-    <row r="70" spans="2:28" s="35" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B70" s="35" t="s">
-        <v>7</v>
-      </c>
-      <c r="N70" s="36">
-        <f>N58+N59</f>
-        <v>319.92399999999998</v>
-      </c>
-      <c r="Q70" s="36">
-        <f t="shared" ref="Q70" si="71">Q58+Q59</f>
-        <v>1005.801</v>
-      </c>
-      <c r="R70" s="36">
-        <f>R58+R59</f>
-        <v>1011.039</v>
-      </c>
-      <c r="S70" s="36">
-        <f>S58+S59</f>
-        <v>1008.296</v>
-      </c>
-      <c r="T70" s="36">
-        <f>T58+T59</f>
-        <v>1005.554</v>
+      <c r="Y70" s="36">
+        <f>F70</f>
+        <v>748.34299999999996</v>
+      </c>
+      <c r="Z70" s="36">
+        <f>J70</f>
+        <v>1812.693</v>
       </c>
       <c r="AA70" s="36">
         <f>N70</f>
-        <v>319.92399999999998</v>
+        <v>3039.7910000000002</v>
       </c>
       <c r="AB70" s="36">
         <f>R70</f>
+        <v>5357.8819999999996</v>
+      </c>
+    </row>
+    <row r="71" spans="2:28" s="35" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B71" s="35" t="s">
+        <v>7</v>
+      </c>
+      <c r="F71" s="36">
+        <f>F59+F60+F56</f>
+        <v>434.49599999999998</v>
+      </c>
+      <c r="J71" s="36">
+        <f>J59+J60+J56</f>
+        <v>473.85999999999996</v>
+      </c>
+      <c r="N71" s="36">
+        <f>N59+N60+N56</f>
+        <v>319.92399999999998</v>
+      </c>
+      <c r="Q71" s="36">
+        <f>Q59+Q60+Q56</f>
+        <v>1005.801</v>
+      </c>
+      <c r="R71" s="36">
+        <f>R59+R60+R56</f>
         <v>1011.039</v>
       </c>
-    </row>
-    <row r="71" spans="2:28" x14ac:dyDescent="0.2">
-      <c r="B71" s="1" t="s">
+      <c r="S71" s="36">
+        <f>S59+S60+S56</f>
+        <v>1008.296</v>
+      </c>
+      <c r="T71" s="36">
+        <f>T59+T60+T56</f>
+        <v>1005.554</v>
+      </c>
+      <c r="Y71" s="36">
+        <f>F71</f>
+        <v>434.49599999999998</v>
+      </c>
+      <c r="Z71" s="36">
+        <f>J71</f>
+        <v>473.85999999999996</v>
+      </c>
+      <c r="AA71" s="36">
+        <f>N71</f>
+        <v>319.92399999999998</v>
+      </c>
+      <c r="AB71" s="36">
+        <f>R71</f>
+        <v>1011.039</v>
+      </c>
+    </row>
+    <row r="72" spans="2:28" x14ac:dyDescent="0.2">
+      <c r="B72" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="N71" s="30">
-        <f t="shared" ref="N71" si="72">N69-N70</f>
+      <c r="F72" s="30">
+        <f t="shared" ref="F72" si="120">F70-F71</f>
+        <v>313.84699999999998</v>
+      </c>
+      <c r="J72" s="30">
+        <f t="shared" ref="J72" si="121">J70-J71</f>
+        <v>1338.8330000000001</v>
+      </c>
+      <c r="N72" s="30">
+        <f t="shared" ref="N72" si="122">N70-N71</f>
         <v>2719.8670000000002</v>
       </c>
-      <c r="Q71" s="30">
-        <f t="shared" ref="Q71" si="73">Q69-Q70</f>
+      <c r="Q72" s="30">
+        <f t="shared" ref="Q72" si="123">Q70-Q71</f>
         <v>4388.451</v>
       </c>
-      <c r="R71" s="30">
-        <f t="shared" ref="R71" si="74">R69-R70</f>
+      <c r="R72" s="30">
+        <f t="shared" ref="R72" si="124">R70-R71</f>
         <v>4346.8429999999998</v>
       </c>
-      <c r="S71" s="30">
-        <f t="shared" ref="S71" si="75">S69-S70</f>
+      <c r="S72" s="30">
+        <f t="shared" ref="S72" si="125">S70-S71</f>
         <v>4215.0159999999996</v>
       </c>
-      <c r="T71" s="30">
-        <f>T69-T70</f>
+      <c r="T72" s="30">
+        <f>T70-T71</f>
         <v>3386.7299999999996</v>
       </c>
-      <c r="AA71" s="30">
-        <f>AA69-AA70</f>
+      <c r="Y72" s="30">
+        <f>Y70-Y71</f>
+        <v>313.84699999999998</v>
+      </c>
+      <c r="Z72" s="30">
+        <f>Z70-Z71</f>
+        <v>1338.8330000000001</v>
+      </c>
+      <c r="AA72" s="30">
+        <f>AA70-AA71</f>
         <v>2719.8670000000002</v>
       </c>
-      <c r="AB71" s="30">
-        <f>AB69-AB70</f>
+      <c r="AB72" s="30">
+        <f>AB70-AB71</f>
         <v>4346.8429999999998</v>
-      </c>
-    </row>
-    <row r="73" spans="2:28" x14ac:dyDescent="0.2">
-      <c r="B73" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="M73" s="1">
-        <v>247.09</v>
-      </c>
-      <c r="N73" s="44">
-        <v>338.5</v>
-      </c>
-      <c r="O73" s="1">
-        <v>340.76</v>
-      </c>
-      <c r="P73" s="1">
-        <v>394.16</v>
-      </c>
-      <c r="Q73" s="1">
-        <v>319.05</v>
-      </c>
-      <c r="R73" s="1">
-        <v>263.33999999999997</v>
-      </c>
-      <c r="S73" s="1">
-        <v>164.81</v>
-      </c>
-      <c r="T73" s="1">
-        <v>83.81</v>
-      </c>
-      <c r="AA73" s="44">
-        <f>N73</f>
-        <v>338.5</v>
-      </c>
-      <c r="AB73" s="1">
-        <f>R73</f>
-        <v>263.33999999999997</v>
       </c>
     </row>
     <row r="74" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B74" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="M74" s="30">
-        <f t="shared" ref="M74:T74" si="76">M73*M17</f>
-        <v>36446.040621749999</v>
-      </c>
-      <c r="N74" s="30">
-        <f t="shared" si="76"/>
-        <v>53612.532779499998</v>
-      </c>
-      <c r="O74" s="30">
-        <f t="shared" si="76"/>
-        <v>56961.597668080001</v>
-      </c>
-      <c r="P74" s="30">
-        <f t="shared" si="76"/>
-        <v>68350.181163679998</v>
-      </c>
-      <c r="Q74" s="30">
-        <f t="shared" si="76"/>
-        <v>56545.641479250007</v>
-      </c>
-      <c r="R74" s="30">
-        <f t="shared" si="76"/>
-        <v>47120.661791279999</v>
-      </c>
-      <c r="S74" s="30">
-        <f t="shared" si="76"/>
-        <v>29813.916889529999</v>
-      </c>
-      <c r="T74" s="30">
-        <f t="shared" si="76"/>
-        <v>15282.57448184</v>
-      </c>
-      <c r="AA74" s="30">
-        <f>AA73*AA17</f>
-        <v>49660.8824255</v>
-      </c>
-      <c r="AB74" s="30">
-        <f>AB73*AB17</f>
-        <v>45868.683653099994</v>
+        <v>3</v>
+      </c>
+      <c r="F74" s="44">
+        <v>89.3</v>
+      </c>
+      <c r="J74" s="44">
+        <v>98.28</v>
+      </c>
+      <c r="M74" s="1">
+        <v>247.09</v>
+      </c>
+      <c r="N74" s="44">
+        <v>338.5</v>
+      </c>
+      <c r="O74" s="1">
+        <v>340.76</v>
+      </c>
+      <c r="P74" s="1">
+        <v>394.16</v>
+      </c>
+      <c r="Q74" s="1">
+        <v>319.05</v>
+      </c>
+      <c r="R74" s="1">
+        <v>263.33999999999997</v>
+      </c>
+      <c r="S74" s="1">
+        <v>164.81</v>
+      </c>
+      <c r="T74" s="1">
+        <v>83.81</v>
+      </c>
+      <c r="Y74" s="44">
+        <v>98.28</v>
+      </c>
+      <c r="Z74" s="44">
+        <v>98.28</v>
+      </c>
+      <c r="AA74" s="44">
+        <f>N74</f>
+        <v>338.5</v>
+      </c>
+      <c r="AB74" s="1">
+        <f>R74</f>
+        <v>263.33999999999997</v>
       </c>
     </row>
     <row r="75" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B75" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F75" s="30">
+        <f t="shared" ref="F75" si="126">F74*F17</f>
+        <v>8878.0191844000001</v>
+      </c>
+      <c r="J75" s="30">
+        <f t="shared" ref="J75" si="127">J74*J17</f>
+        <v>13535.96464584</v>
+      </c>
+      <c r="M75" s="30">
+        <f t="shared" ref="M75:T75" si="128">M74*M17</f>
+        <v>36446.040621749999</v>
+      </c>
+      <c r="N75" s="30">
+        <f t="shared" si="128"/>
+        <v>53612.532779499998</v>
+      </c>
+      <c r="O75" s="30">
+        <f t="shared" si="128"/>
+        <v>56961.597668080001</v>
+      </c>
+      <c r="P75" s="30">
+        <f t="shared" si="128"/>
+        <v>68350.181163679998</v>
+      </c>
+      <c r="Q75" s="30">
+        <f t="shared" si="128"/>
+        <v>56545.641479250007</v>
+      </c>
+      <c r="R75" s="30">
+        <f t="shared" si="128"/>
+        <v>47120.661791279999</v>
+      </c>
+      <c r="S75" s="30">
+        <f t="shared" si="128"/>
+        <v>29813.916889529999</v>
+      </c>
+      <c r="T75" s="30">
+        <f t="shared" si="128"/>
+        <v>15282.57448184</v>
+      </c>
+      <c r="Y75" s="30">
+        <f t="shared" ref="Y75" si="129">Y74*Y17</f>
+        <v>9545.9697169200008</v>
+      </c>
+      <c r="Z75" s="30">
+        <f>Z74*Z17</f>
+        <v>12784.56176088</v>
+      </c>
+      <c r="AA75" s="30">
+        <f>AA74*AA17</f>
+        <v>49660.8824255</v>
+      </c>
+      <c r="AB75" s="30">
+        <f>AB74*AB17</f>
+        <v>45868.683653099994</v>
+      </c>
+    </row>
+    <row r="76" spans="2:28" x14ac:dyDescent="0.2">
+      <c r="B76" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="N75" s="30">
-        <f t="shared" ref="N75" si="77">N74-N71</f>
+      <c r="F76" s="30">
+        <f t="shared" ref="F76" si="130">F75-F72</f>
+        <v>8564.1721844000003</v>
+      </c>
+      <c r="J76" s="30">
+        <f t="shared" ref="J76" si="131">J75-J72</f>
+        <v>12197.13164584</v>
+      </c>
+      <c r="N76" s="30">
+        <f t="shared" ref="N76" si="132">N75-N72</f>
         <v>50892.665779499999</v>
       </c>
-      <c r="P75" s="30"/>
-      <c r="Q75" s="30"/>
-      <c r="R75" s="30">
-        <f t="shared" ref="R75" si="78">R74-R71</f>
+      <c r="P76" s="30"/>
+      <c r="Q76" s="30">
+        <f t="shared" ref="Q76:R76" si="133">Q75-Q72</f>
+        <v>52157.190479250006</v>
+      </c>
+      <c r="R76" s="30">
+        <f t="shared" si="133"/>
         <v>42773.818791279999</v>
       </c>
-      <c r="S75" s="30">
-        <f t="shared" ref="S75" si="79">S74-S71</f>
+      <c r="S76" s="30">
+        <f t="shared" ref="S76" si="134">S75-S72</f>
         <v>25598.900889529999</v>
       </c>
-      <c r="T75" s="30">
-        <f>T74-T71</f>
+      <c r="T76" s="30">
+        <f>T75-T72</f>
         <v>11895.84448184</v>
       </c>
-      <c r="AA75" s="30">
-        <f t="shared" ref="AA75" si="80">AA74-AA71</f>
+      <c r="Y76" s="30">
+        <f t="shared" ref="Y76:Z76" si="135">Y75-Y72</f>
+        <v>9232.122716920001</v>
+      </c>
+      <c r="Z76" s="30">
+        <f t="shared" ref="Z76:AA76" si="136">Z75-Z72</f>
+        <v>11445.72876088</v>
+      </c>
+      <c r="AA76" s="30">
+        <f t="shared" si="136"/>
         <v>46941.015425500002</v>
       </c>
-      <c r="AB75" s="30">
-        <f t="shared" ref="AB75" si="81">AB74-AB71</f>
+      <c r="AB76" s="30">
+        <f t="shared" ref="AB76" si="137">AB75-AB72</f>
         <v>41521.840653099993</v>
-      </c>
-    </row>
-    <row r="77" spans="2:28" x14ac:dyDescent="0.2">
-      <c r="B77" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="N77" s="37">
-        <f>N73/N67</f>
-        <v>6.3426780523657325</v>
-      </c>
-      <c r="Q77" s="37">
-        <f t="shared" ref="Q77" si="82">Q73/Q67</f>
-        <v>5.1025917911739382</v>
-      </c>
-      <c r="R77" s="37">
-        <f>R73/R67</f>
-        <v>4.2714777701603754</v>
-      </c>
-      <c r="S77" s="37">
-        <f>S73/S67</f>
-        <v>2.730854120151688</v>
-      </c>
-      <c r="T77" s="37">
-        <f>T73/T67</f>
-        <v>1.4095721757702342</v>
-      </c>
-      <c r="AA77" s="37">
-        <f>AA73/AA67</f>
-        <v>5.8751745663054189</v>
-      </c>
-      <c r="AB77" s="37">
-        <f>AB73/AB67</f>
-        <v>4.1579862235082805</v>
       </c>
     </row>
     <row r="78" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B78" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
+      </c>
+      <c r="F78" s="37">
+        <f>F74/F68</f>
+        <v>20.258580862779098</v>
+      </c>
+      <c r="J78" s="37">
+        <f>J74/J68</f>
+        <v>3.1778958747676609</v>
       </c>
       <c r="N78" s="37">
-        <f t="shared" ref="N78" si="83">N74/SUM(K4:N4)</f>
-        <v>53.82465574780209</v>
+        <f>N74/N68</f>
+        <v>6.3426780523657325</v>
       </c>
       <c r="Q78" s="37">
-        <f t="shared" ref="Q78" si="84">Q74/SUM(N4:Q4)</f>
-        <v>22.199267614739412</v>
+        <f t="shared" ref="Q78" si="138">Q74/Q68</f>
+        <v>5.1026746735277291</v>
       </c>
       <c r="R78" s="37">
-        <f t="shared" ref="R78:S78" si="85">R74/SUM(O4:R4)</f>
-        <v>16.581045510065838</v>
+        <f>R74/R68</f>
+        <v>4.2714777701603754</v>
       </c>
       <c r="S78" s="37">
-        <f t="shared" si="85"/>
-        <v>9.5336989696036145</v>
+        <f>S74/S68</f>
+        <v>2.730854120151688</v>
       </c>
       <c r="T78" s="37">
-        <f>T74/SUM(Q4:T4)</f>
-        <v>4.4927117390362339</v>
+        <f>T74/T68</f>
+        <v>1.4095721757702342</v>
+      </c>
+      <c r="Y78" s="37">
+        <f t="shared" ref="Y78:Z78" si="139">Y74/Y68</f>
+        <v>21.782764308921006</v>
+      </c>
+      <c r="Z78" s="37">
+        <f t="shared" ref="Z78:AA78" si="140">Z74/Z68</f>
+        <v>3.0124374838015551</v>
       </c>
       <c r="AA78" s="37">
-        <f>AA74/AA4</f>
-        <v>28.187966248546921</v>
+        <f>AA74/AA68</f>
+        <v>5.8751745663054189</v>
       </c>
       <c r="AB78" s="37">
-        <f>AB74/AB4</f>
-        <v>16.140493410464138</v>
+        <f>AB74/AB68</f>
+        <v>4.1579862235082805</v>
       </c>
     </row>
     <row r="79" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B79" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="N79" s="37">
+        <f t="shared" ref="N79" si="141">N75/SUM(K4:N4)</f>
+        <v>53.82465574780209</v>
+      </c>
+      <c r="Q79" s="37">
+        <f t="shared" ref="Q79" si="142">Q75/SUM(N4:Q4)</f>
+        <v>22.199267614739412</v>
+      </c>
+      <c r="R79" s="37">
+        <f t="shared" ref="R79:S79" si="143">R75/SUM(O4:R4)</f>
+        <v>16.581045510065838</v>
+      </c>
+      <c r="S79" s="37">
+        <f t="shared" si="143"/>
+        <v>9.5336989696036145</v>
+      </c>
+      <c r="T79" s="37">
+        <f>T75/SUM(Q4:T4)</f>
+        <v>4.4927117390362339</v>
+      </c>
+      <c r="Y79" s="37">
+        <f t="shared" ref="Y79:Z79" si="144">Y75/Y4</f>
+        <v>14.684593614073627</v>
+      </c>
+      <c r="Z79" s="37">
+        <f t="shared" ref="Z79:AA79" si="145">Z75/Z4</f>
+        <v>11.269213200266556</v>
+      </c>
+      <c r="AA79" s="37">
+        <f>AA75/AA4</f>
+        <v>28.187966248546921</v>
+      </c>
+      <c r="AB79" s="37">
+        <f>AB75/AB4</f>
+        <v>16.140493410464138</v>
+      </c>
+    </row>
+    <row r="80" spans="2:28" x14ac:dyDescent="0.2">
+      <c r="B80" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="N79" s="37">
-        <f t="shared" ref="N79" si="86">N73/SUM(K16:N16)</f>
+      <c r="N80" s="37">
+        <f t="shared" ref="N80" si="146">N74/SUM(K16:N16)</f>
         <v>-175.84216103089744</v>
       </c>
-      <c r="Q79" s="37">
-        <f t="shared" ref="Q79" si="87">Q73/SUM(N16:Q16)</f>
+      <c r="Q80" s="37">
+        <f t="shared" ref="Q80" si="147">Q74/SUM(N16:Q16)</f>
         <v>-64.500694009685063</v>
       </c>
-      <c r="R79" s="37">
-        <f t="shared" ref="R79:S79" si="88">R73/SUM(O16:R16)</f>
+      <c r="R80" s="37">
+        <f t="shared" ref="R80:S80" si="148">R74/SUM(O16:R16)</f>
         <v>-48.385204422553002</v>
       </c>
-      <c r="S79" s="37">
-        <f t="shared" si="88"/>
+      <c r="S80" s="37">
+        <f t="shared" si="148"/>
         <v>-30.339872026893296</v>
       </c>
-      <c r="T79" s="37">
-        <f>T73/SUM(Q16:T16)</f>
+      <c r="T80" s="37">
+        <f>T74/SUM(Q16:T16)</f>
         <v>-14.233498713981406</v>
       </c>
-      <c r="AA79" s="37">
-        <f>AA73/AA16</f>
+      <c r="Y80" s="37">
+        <f t="shared" ref="Y80:AA80" si="149">Y74/Y16</f>
+        <v>-78.278376345193479</v>
+      </c>
+      <c r="Z80" s="37">
+        <f t="shared" si="149"/>
+        <v>-41.634979665019884</v>
+      </c>
+      <c r="AA80" s="37">
+        <f>AA74/AA16</f>
         <v>-101.14665276009771</v>
       </c>
-      <c r="AB79" s="37">
-        <f>AB73/AB16</f>
+      <c r="AB80" s="37">
+        <f>AB74/AB16</f>
         <v>-48.287907835666907</v>
       </c>
     </row>
@@ -14519,14 +15552,18 @@
     <hyperlink ref="R1" r:id="rId3" xr:uid="{A293EABB-9A75-4B29-8553-BB352A36DBB6}"/>
     <hyperlink ref="AB1" r:id="rId4" xr:uid="{442A1034-B338-4801-AF1E-61BA7E0E77AC}"/>
     <hyperlink ref="Q1" r:id="rId5" xr:uid="{BA74861F-598C-41FE-BE22-C6AA1B8966A6}"/>
+    <hyperlink ref="Z1" r:id="rId6" xr:uid="{4D41E43B-78DD-4BC7-9AA5-4C75C95D3E6E}"/>
+    <hyperlink ref="Y1" r:id="rId7" xr:uid="{620C08C8-E4C1-490D-823F-7D8C45A07CBD}"/>
+    <hyperlink ref="J1" r:id="rId8" xr:uid="{A20F0590-51BB-47FE-A2F0-ABB514CD183A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="256" orientation="portrait" horizontalDpi="203" verticalDpi="203" r:id="rId6"/>
+  <pageSetup paperSize="256" orientation="portrait" horizontalDpi="203" verticalDpi="203" r:id="rId9"/>
   <ignoredErrors>
-    <ignoredError sqref="AA44:AB44 AA56:AB56" formula="1"/>
-    <ignoredError sqref="N78:P78 S78:T78 Q78:R78" formulaRange="1"/>
+    <ignoredError sqref="Y44:AB44 Y58:AB62 Y50 AA50:AB50 Y48:AB49 Y47 AA47:AB47 Y46:AB46 Y45 AA45:AB45 Y51:AB55 U57:X57 Y57:AB57" formula="1"/>
+    <ignoredError sqref="N79:P79 S79:T79 Q79:R79" formulaRange="1"/>
   </ignoredErrors>
-  <drawing r:id="rId7"/>
+  <drawing r:id="rId10"/>
+  <legacyDrawing r:id="rId11"/>
 </worksheet>
 </file>
 
@@ -14534,8 +15571,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33C88468-B575-4B07-B1E2-1E3BE5EA25D5}">
   <dimension ref="A1:G1596"/>
   <sheetViews>
-    <sheetView topLeftCell="A1016" workbookViewId="0">
-      <selection activeCell="F1046" sqref="F1046"/>
+    <sheetView topLeftCell="A866" workbookViewId="0">
+      <selection activeCell="A888" sqref="A888"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>

</xml_diff>